<commit_message>
om shanti mandir estimate continue with provisional sum added but still not complete and postponed for till meeting with plumber
</commit_message>
<xml_diff>
--- a/ofc/estimates/Om shanti mandir/ૐ शान्ति भवन निर्माण तथा मर्मत.xlsx
+++ b/ofc/estimates/Om shanti mandir/ૐ शान्ति भवन निर्माण तथा मर्मत.xlsx
@@ -36,7 +36,7 @@
     <definedName name="description_6">[3]Abstract!$B$172</definedName>
     <definedName name="description_759">[1]Abstract!$B$278</definedName>
     <definedName name="description_783">[1]Abstract!$B$301</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Sheet4 (2)'!$A$1:$K$42</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Sheet4 (2)'!$A$1:$K$44</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Sheet4 (2)'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">WCR!$1:$12</definedName>
   </definedNames>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>Porcelain clay white glaze wash basin (500*400)mm size regular</t>
+  </si>
+  <si>
+    <t>Provisional sum for unforseen works</t>
   </si>
 </sst>
 </file>
@@ -575,81 +578,81 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1230,90 +1233,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="I1" s="77"/>
+      <c r="J1" s="77"/>
+      <c r="K1" s="77"/>
     </row>
     <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
-      <c r="E2" s="72"/>
-      <c r="F2" s="72"/>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
+      <c r="B2" s="78"/>
+      <c r="C2" s="78"/>
+      <c r="D2" s="78"/>
+      <c r="E2" s="78"/>
+      <c r="F2" s="78"/>
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="80" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="73"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
+      <c r="E5" s="80"/>
+      <c r="F5" s="80"/>
+      <c r="G5" s="80"/>
+      <c r="H5" s="80"/>
+      <c r="I5" s="80"/>
+      <c r="J5" s="80"/>
+      <c r="K5" s="80"/>
     </row>
     <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="69" t="e">
+      <c r="C6" s="75" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="70"/>
+      <c r="D6" s="76"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -1321,11 +1324,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="69" t="e">
+      <c r="J6" s="75" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="70"/>
+      <c r="K6" s="76"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
@@ -1334,77 +1337,77 @@
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="I7" s="77" t="s">
+      <c r="F7" s="70"/>
+      <c r="G7" s="70"/>
+      <c r="I7" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
+      <c r="J7" s="71"/>
+      <c r="K7" s="71"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="63" t="e">
+      <c r="A8" s="69" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="63"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="I8" s="78" t="s">
+      <c r="B8" s="69"/>
+      <c r="C8" s="69"/>
+      <c r="D8" s="69"/>
+      <c r="E8" s="69"/>
+      <c r="F8" s="69"/>
+      <c r="I8" s="72" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
+      <c r="J8" s="72"/>
+      <c r="K8" s="72"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="79" t="e">
+      <c r="A9" s="73" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="I9" s="78" t="s">
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="I9" s="72" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
+      <c r="J9" s="72"/>
+      <c r="K9" s="72"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="74" t="s">
+      <c r="A11" s="67" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="74" t="s">
+      <c r="C11" s="67" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="80" t="s">
+      <c r="D11" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="80" t="s">
+      <c r="E11" s="74"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="80"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="74" t="s">
+      <c r="H11" s="74"/>
+      <c r="I11" s="74"/>
+      <c r="J11" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="75" t="s">
+      <c r="K11" s="68" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="74"/>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
+      <c r="A12" s="67"/>
+      <c r="B12" s="67"/>
+      <c r="C12" s="67"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -1423,8 +1426,8 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="74"/>
-      <c r="K12" s="75"/>
+      <c r="J12" s="67"/>
+      <c r="K12" s="68"/>
     </row>
     <row r="13" spans="1:11" s="1" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="e">
@@ -1586,6 +1589,13 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -1599,13 +1609,6 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1621,10 +1624,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S99"/>
+  <dimension ref="A1:S101"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1642,113 +1645,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="65" t="s">
+      <c r="A1" s="86" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
-      <c r="E1" s="65"/>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="65"/>
-      <c r="I1" s="65"/>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
     </row>
     <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="66"/>
-      <c r="E2" s="66"/>
-      <c r="F2" s="66"/>
-      <c r="G2" s="66"/>
-      <c r="H2" s="66"/>
-      <c r="I2" s="66"/>
-      <c r="J2" s="66"/>
-      <c r="K2" s="66"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
+      <c r="J2" s="87"/>
+      <c r="K2" s="87"/>
     </row>
     <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67" t="s">
+      <c r="A3" s="79" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-      <c r="G3" s="67"/>
-      <c r="H3" s="67"/>
-      <c r="I3" s="67"/>
-      <c r="J3" s="67"/>
-      <c r="K3" s="67"/>
+      <c r="B3" s="79"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
     </row>
     <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="79" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
-      <c r="H4" s="67"/>
-      <c r="I4" s="67"/>
-      <c r="J4" s="67"/>
-      <c r="K4" s="67"/>
+      <c r="B4" s="79"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
     </row>
     <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="68" t="s">
+      <c r="A5" s="88" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="68"/>
-      <c r="C5" s="68"/>
-      <c r="D5" s="68"/>
-      <c r="E5" s="68"/>
-      <c r="F5" s="68"/>
-      <c r="G5" s="68"/>
-      <c r="H5" s="68"/>
-      <c r="I5" s="68"/>
-      <c r="J5" s="68"/>
-      <c r="K5" s="68"/>
+      <c r="B5" s="88"/>
+      <c r="C5" s="88"/>
+      <c r="D5" s="88"/>
+      <c r="E5" s="88"/>
+      <c r="F5" s="88"/>
+      <c r="G5" s="88"/>
+      <c r="H5" s="88"/>
+      <c r="I5" s="88"/>
+      <c r="J5" s="88"/>
+      <c r="K5" s="88"/>
     </row>
     <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="69" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
+      <c r="B6" s="69"/>
+      <c r="C6" s="69"/>
+      <c r="D6" s="69"/>
+      <c r="E6" s="69"/>
+      <c r="F6" s="69"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="64" t="s">
+      <c r="H6" s="85" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="64"/>
-      <c r="J6" s="64"/>
-      <c r="K6" s="64"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
     </row>
     <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="81" t="s">
+      <c r="A7" s="82" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="81"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="81"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
+      <c r="B7" s="82"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="82" t="s">
+      <c r="H7" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
     </row>
     <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
@@ -1786,13 +1789,13 @@
       </c>
     </row>
     <row r="9" spans="1:19" s="1" customFormat="1" ht="54.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="85">
+      <c r="A9" s="63">
         <v>1</v>
       </c>
-      <c r="B9" s="86" t="s">
+      <c r="B9" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="86"/>
+      <c r="C9" s="64"/>
       <c r="D9" s="40"/>
       <c r="E9" s="40"/>
       <c r="F9" s="40"/>
@@ -2038,7 +2041,7 @@
       <c r="A18" s="18">
         <v>2</v>
       </c>
-      <c r="B18" s="87" t="s">
+      <c r="B18" s="65" t="s">
         <v>51</v>
       </c>
       <c r="C18" s="37"/>
@@ -2166,7 +2169,7 @@
       <c r="A23" s="18">
         <v>3</v>
       </c>
-      <c r="B23" s="88" t="s">
+      <c r="B23" s="66" t="s">
         <v>53</v>
       </c>
       <c r="C23" s="29"/>
@@ -2174,8 +2177,8 @@
       <c r="E23" s="40"/>
       <c r="F23" s="40"/>
       <c r="G23" s="40"/>
-      <c r="H23" s="85"/>
-      <c r="I23" s="85"/>
+      <c r="H23" s="63"/>
+      <c r="I23" s="63"/>
       <c r="J23" s="45"/>
       <c r="K23" s="21"/>
       <c r="M23" s="35"/>
@@ -2290,7 +2293,7 @@
       <c r="A28" s="18">
         <v>4</v>
       </c>
-      <c r="B28" s="88" t="s">
+      <c r="B28" s="66" t="s">
         <v>55</v>
       </c>
       <c r="C28" s="29"/>
@@ -2298,8 +2301,8 @@
       <c r="E28" s="40"/>
       <c r="F28" s="40"/>
       <c r="G28" s="40"/>
-      <c r="H28" s="85"/>
-      <c r="I28" s="85"/>
+      <c r="H28" s="63"/>
+      <c r="I28" s="63"/>
       <c r="J28" s="45"/>
       <c r="K28" s="21"/>
       <c r="M28" s="35"/>
@@ -2391,24 +2394,31 @@
       <c r="S31" s="25"/>
     </row>
     <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="41"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="38"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="44"/>
-      <c r="E32" s="44"/>
-      <c r="F32" s="44"/>
-      <c r="G32" s="44"/>
-      <c r="H32" s="44"/>
-      <c r="I32" s="44"/>
+      <c r="C32" s="37"/>
+      <c r="D32" s="39"/>
+      <c r="E32" s="39"/>
+      <c r="F32" s="39"/>
+      <c r="G32" s="40"/>
+      <c r="H32" s="41"/>
+      <c r="I32" s="41"/>
       <c r="J32" s="45"/>
-      <c r="K32" s="37"/>
-    </row>
-    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K32" s="21"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="25"/>
+      <c r="S32" s="25"/>
+    </row>
+    <row r="33" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="18">
         <v>5</v>
       </c>
       <c r="B33" s="30" t="s">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="C33" s="19">
         <v>1</v>
@@ -2424,11 +2434,11 @@
         <v>31</v>
       </c>
       <c r="I33" s="23">
-        <v>500</v>
+        <v>20000</v>
       </c>
       <c r="J33" s="34">
         <f>G33*I33</f>
-        <v>500</v>
+        <v>20000</v>
       </c>
       <c r="K33" s="21"/>
       <c r="M33" s="25"/>
@@ -2440,128 +2450,135 @@
       <c r="S33" s="25"/>
     </row>
     <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="18"/>
-      <c r="B34" s="24"/>
-      <c r="C34" s="19"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="21"/>
-      <c r="F34" s="21"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="22"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="42"/>
-      <c r="K34" s="21"/>
-      <c r="M34" s="25"/>
-      <c r="N34" s="1"/>
-      <c r="O34" s="1"/>
-      <c r="P34" s="1"/>
-      <c r="Q34" s="1"/>
-      <c r="R34" s="25"/>
-      <c r="S34" s="25"/>
-    </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35" s="41"/>
-      <c r="B35" s="46" t="s">
+      <c r="A34" s="41"/>
+      <c r="B34" s="38"/>
+      <c r="C34" s="43"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="44"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="44"/>
+      <c r="H34" s="44"/>
+      <c r="I34" s="44"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="37"/>
+    </row>
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="18">
+        <v>5</v>
+      </c>
+      <c r="B35" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="19">
+        <v>1</v>
+      </c>
+      <c r="D35" s="20"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="34">
+        <f t="shared" ref="G35" si="5">PRODUCT(C35:F35)</f>
+        <v>1</v>
+      </c>
+      <c r="H35" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I35" s="23">
+        <v>500</v>
+      </c>
+      <c r="J35" s="34">
+        <f>G35*I35</f>
+        <v>500</v>
+      </c>
+      <c r="K35" s="21"/>
+      <c r="M35" s="25"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="25"/>
+      <c r="S35" s="25"/>
+    </row>
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="18"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="19"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="23"/>
+      <c r="H36" s="22"/>
+      <c r="I36" s="23"/>
+      <c r="J36" s="42"/>
+      <c r="K36" s="21"/>
+      <c r="M36" s="25"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="25"/>
+      <c r="S36" s="25"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A37" s="41"/>
+      <c r="B37" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C35" s="47"/>
-      <c r="D35" s="39"/>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
-      <c r="G35" s="42"/>
-      <c r="H35" s="42"/>
-      <c r="I35" s="42"/>
-      <c r="J35" s="42">
-        <f>SUM(J9:J33)</f>
-        <v>83926.718339093713</v>
-      </c>
-      <c r="K35" s="37"/>
-    </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36" s="58"/>
-      <c r="B36" s="61"/>
-      <c r="C36" s="62"/>
-      <c r="D36" s="59"/>
-      <c r="E36" s="59"/>
-      <c r="F36" s="59"/>
-      <c r="G36" s="60"/>
-      <c r="H36" s="60"/>
-      <c r="I36" s="60"/>
-      <c r="J36" s="60"/>
-      <c r="K36" s="57"/>
-    </row>
-    <row r="37" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="50"/>
-      <c r="B37" s="29" t="s">
+      <c r="C37" s="47"/>
+      <c r="D37" s="39"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
+      <c r="G37" s="42"/>
+      <c r="H37" s="42"/>
+      <c r="I37" s="42"/>
+      <c r="J37" s="42">
+        <f>SUM(J9:J35)</f>
+        <v>103926.71833909371</v>
+      </c>
+      <c r="K37" s="37"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A38" s="58"/>
+      <c r="B38" s="61"/>
+      <c r="C38" s="62"/>
+      <c r="D38" s="59"/>
+      <c r="E38" s="59"/>
+      <c r="F38" s="59"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="57"/>
+    </row>
+    <row r="39" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="50"/>
+      <c r="B39" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="83">
-        <f>J35</f>
-        <v>83926.718339093713</v>
-      </c>
-      <c r="D37" s="83"/>
-      <c r="E37" s="40">
+      <c r="C39" s="81">
+        <f>J37</f>
+        <v>103926.71833909371</v>
+      </c>
+      <c r="D39" s="81"/>
+      <c r="E39" s="40">
         <v>100</v>
       </c>
-      <c r="F37" s="51"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="51"/>
-      <c r="I37" s="53"/>
-      <c r="J37" s="54"/>
-      <c r="K37" s="55"/>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="56"/>
-      <c r="B38" s="29" t="s">
-        <v>32</v>
-      </c>
-      <c r="C38" s="84">
-        <v>100000</v>
-      </c>
-      <c r="D38" s="84"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="49"/>
-      <c r="G38" s="48"/>
-      <c r="H38" s="48"/>
-      <c r="I38" s="48"/>
-      <c r="J38" s="48"/>
-      <c r="K38" s="49"/>
-    </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39" s="56"/>
-      <c r="B39" s="29" t="s">
-        <v>33</v>
-      </c>
-      <c r="C39" s="84">
-        <f>C38-C41-C42</f>
-        <v>95000</v>
-      </c>
-      <c r="D39" s="84"/>
-      <c r="E39" s="40">
-        <f>C39/C37*100</f>
-        <v>113.19398861297817</v>
-      </c>
-      <c r="F39" s="49"/>
-      <c r="G39" s="48"/>
-      <c r="H39" s="48"/>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
-      <c r="K39" s="49"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="51"/>
+      <c r="I39" s="53"/>
+      <c r="J39" s="54"/>
+      <c r="K39" s="55"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40" s="56"/>
       <c r="B40" s="29" t="s">
-        <v>34</v>
-      </c>
-      <c r="C40" s="83">
-        <f>C37-C39</f>
-        <v>-11073.281660906287</v>
-      </c>
-      <c r="D40" s="83"/>
-      <c r="E40" s="40">
-        <f>100-E39</f>
-        <v>-13.193988612978174</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="C40" s="84">
+        <v>100000</v>
+      </c>
+      <c r="D40" s="84"/>
+      <c r="E40" s="40"/>
       <c r="F40" s="49"/>
       <c r="G40" s="48"/>
       <c r="H40" s="48"/>
@@ -2572,15 +2589,16 @@
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41" s="56"/>
       <c r="B41" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C41" s="83">
-        <f>C38*0.03</f>
-        <v>3000</v>
-      </c>
-      <c r="D41" s="83"/>
+        <v>33</v>
+      </c>
+      <c r="C41" s="84">
+        <f>C40-C43-C44</f>
+        <v>95000</v>
+      </c>
+      <c r="D41" s="84"/>
       <c r="E41" s="40">
-        <v>3</v>
+        <f>C41/C39*100</f>
+        <v>91.410564596134478</v>
       </c>
       <c r="F41" s="49"/>
       <c r="G41" s="48"/>
@@ -2592,15 +2610,16 @@
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42" s="56"/>
       <c r="B42" s="29" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="83">
-        <f>C38*0.02</f>
-        <v>2000</v>
-      </c>
-      <c r="D42" s="83"/>
+        <v>34</v>
+      </c>
+      <c r="C42" s="81">
+        <f>C39-C41</f>
+        <v>8926.7183390937134</v>
+      </c>
+      <c r="D42" s="81"/>
       <c r="E42" s="40">
-        <v>2</v>
+        <f>100-E41</f>
+        <v>8.5894354038655223</v>
       </c>
       <c r="F42" s="49"/>
       <c r="G42" s="48"/>
@@ -2609,21 +2628,59 @@
       <c r="J42" s="48"/>
       <c r="K42" s="49"/>
     </row>
-    <row r="43" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="57"/>
-      <c r="B43" s="57"/>
-      <c r="C43" s="57"/>
-      <c r="D43" s="57"/>
-      <c r="E43" s="57"/>
-      <c r="F43" s="57"/>
-      <c r="G43" s="57"/>
-      <c r="H43" s="57"/>
-      <c r="I43" s="57"/>
-      <c r="J43" s="57"/>
-      <c r="K43" s="57"/>
-    </row>
-    <row r="44" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A43" s="56"/>
+      <c r="B43" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C43" s="81">
+        <f>C40*0.03</f>
+        <v>3000</v>
+      </c>
+      <c r="D43" s="81"/>
+      <c r="E43" s="40">
+        <v>3</v>
+      </c>
+      <c r="F43" s="49"/>
+      <c r="G43" s="48"/>
+      <c r="H43" s="48"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
+      <c r="K43" s="49"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A44" s="56"/>
+      <c r="B44" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="81">
+        <f>C40*0.02</f>
+        <v>2000</v>
+      </c>
+      <c r="D44" s="81"/>
+      <c r="E44" s="40">
+        <v>2</v>
+      </c>
+      <c r="F44" s="49"/>
+      <c r="G44" s="48"/>
+      <c r="H44" s="48"/>
+      <c r="I44" s="48"/>
+      <c r="J44" s="48"/>
+      <c r="K44" s="49"/>
+    </row>
+    <row r="45" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="57"/>
+      <c r="B45" s="57"/>
+      <c r="C45" s="57"/>
+      <c r="D45" s="57"/>
+      <c r="E45" s="57"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57"/>
+      <c r="H45" s="57"/>
+      <c r="I45" s="57"/>
+      <c r="J45" s="57"/>
+      <c r="K45" s="57"/>
+    </row>
     <row r="46" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="47" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -2678,16 +2735,10 @@
     <row r="97" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="98" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="99" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C37:D37"/>
-    <mergeCell ref="C38:D38"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -2695,6 +2746,14 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
+    <mergeCell ref="C43:D43"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C39:D39"/>
+    <mergeCell ref="C40:D40"/>
+    <mergeCell ref="C41:D41"/>
+    <mergeCell ref="C42:D42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
om shanti mandir estimate complete and pashikhel estimate partial done
</commit_message>
<xml_diff>
--- a/ofc/estimates/Om shanti mandir/ૐ शान्ति भवन निर्माण तथा मर्मत.xlsx
+++ b/ofc/estimates/Om shanti mandir/ૐ शान्ति भवन निर्माण तथा मर्मत.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\Om shanti mandir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\Om shanti mandir\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WCR" sheetId="6" r:id="rId1"/>
@@ -36,11 +36,11 @@
     <definedName name="description_6">[3]Abstract!$B$172</definedName>
     <definedName name="description_759">[1]Abstract!$B$278</definedName>
     <definedName name="description_783">[1]Abstract!$B$301</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'Sheet4 (2)'!$A$1:$K$44</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'Sheet4 (2)'!$A$1:$K$89</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Sheet4 (2)'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -57,8 +57,306 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>DELL</author>
+  </authors>
+  <commentList>
+    <comment ref="I15" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>DELL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Item 134 from civil rate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I20" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>DELL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+PG .No. 165 ktm jilla darr rate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>DELL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+PG No. 169 ktm jilla darr rate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I30" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>DELL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+White cement per 40kg bag rs 1230 PG.no.18 Ktm jilla darr rate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I35" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>DELL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+PG .No. 165 ktm jilla darr rate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I40" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>DELL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+PG. No. 166 ktm jilla darr rate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I45" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>DELL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+PG. No. 169 ktm jilla darr rate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I50" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>DELL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+PG. No. 169 ktm jilla darr rate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I55" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>DELL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+PG. No. 169 ktm jilla darr rate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I60" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>DELL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+PG. No. 169 ktm jilla darr rate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I65" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>DELL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+PG. No. 151 ktm jilla darr rate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I70" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>DELL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+PG. No. 151 ktm jilla darr rate</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I75" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t>DELL:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+          </rPr>
+          <t xml:space="preserve">
+PG. No. 151 ktm jilla darr rate</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="77">
   <si>
     <t>Government of Nepal</t>
   </si>
@@ -232,33 +530,93 @@
     <t>-deduction for overlap</t>
   </si>
   <si>
-    <t>White glazed porcelain clay one piece commode with 'P' and 'S' trap and slow falling seat cover complete set</t>
-  </si>
-  <si>
     <t>-commode for toilet</t>
   </si>
   <si>
-    <t>600mm to 900mm grab bar</t>
-  </si>
-  <si>
-    <t>-for toilet</t>
-  </si>
-  <si>
-    <t>Porcelain clay white glaze wash basin (500*400)mm size regular</t>
-  </si>
-  <si>
     <t>Provisional sum for unforseen works</t>
+  </si>
+  <si>
+    <t>-for commode</t>
+  </si>
+  <si>
+    <t>White cement for fixtures</t>
+  </si>
+  <si>
+    <t>-white cement</t>
+  </si>
+  <si>
+    <t>Kg</t>
+  </si>
+  <si>
+    <t>piece</t>
+  </si>
+  <si>
+    <t>-for hand washing</t>
+  </si>
+  <si>
+    <t>-for basin</t>
+  </si>
+  <si>
+    <t>-for bathroom/toilet</t>
+  </si>
+  <si>
+    <t>-for bathroom</t>
+  </si>
+  <si>
+    <t>-for kitchen</t>
+  </si>
+  <si>
+    <t>-fittings</t>
+  </si>
+  <si>
+    <t>-45cm long bend type</t>
+  </si>
+  <si>
+    <t>-European pattern C.P Grab Bar for disable all complete set</t>
+  </si>
+  <si>
+    <t>Stainless steel commode spray with hose pipe all complete set</t>
+  </si>
+  <si>
+    <t>White glazed porcelain clay one piece commode with 'P' and 'S' trap and slow falling seat cover all complete set</t>
+  </si>
+  <si>
+    <t>Porcelain clay white glaze wash basin (500*400)mm size regular all complete set</t>
+  </si>
+  <si>
+    <t>Stainless steel single faucet for basin mixture all complete set</t>
+  </si>
+  <si>
+    <t>Looking Mirror Modi Guard 450*600mm (18"*24") all complete set</t>
+  </si>
+  <si>
+    <t>Wall Mixer shower faucet ( conceal system) all complete set</t>
+  </si>
+  <si>
+    <t>Stainless steel kitchen sink mixture all complete set</t>
+  </si>
+  <si>
+    <t>CP Toilet paper holder all complete set</t>
+  </si>
+  <si>
+    <t>Towel rod 1/2" *18" all complete set</t>
+  </si>
+  <si>
+    <t>Glass shelf all complete set</t>
+  </si>
+  <si>
+    <t>Item 134 from civil rate</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -376,6 +734,30 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -397,7 +779,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -429,12 +811,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="89">
+  <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -442,7 +861,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -462,14 +881,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -478,7 +897,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -503,7 +922,7 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -538,7 +957,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -546,7 +965,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -561,7 +980,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -577,7 +996,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -590,6 +1009,24 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -614,22 +1051,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -642,17 +1073,20 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="13" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1217,106 +1651,106 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.28515625" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="8.85546875" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.33203125" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="77" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-    </row>
-    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="78" t="s">
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+    </row>
+    <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
+      <c r="A2" s="70" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="78"/>
-      <c r="C2" s="78"/>
-      <c r="D2" s="78"/>
-      <c r="E2" s="78"/>
-      <c r="F2" s="78"/>
-      <c r="G2" s="78"/>
-      <c r="H2" s="78"/>
-      <c r="I2" s="78"/>
-      <c r="J2" s="78"/>
-      <c r="K2" s="78"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79" t="s">
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-    </row>
-    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="80" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+    </row>
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="72" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
-      <c r="E5" s="80"/>
-      <c r="F5" s="80"/>
-      <c r="G5" s="80"/>
-      <c r="H5" s="80"/>
-      <c r="I5" s="80"/>
-      <c r="J5" s="80"/>
-      <c r="K5" s="80"/>
-    </row>
-    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B5" s="72"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="72"/>
+      <c r="J5" s="72"/>
+      <c r="K5" s="72"/>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="75" t="e">
+      <c r="C6" s="67" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="76"/>
+      <c r="D6" s="68"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -1324,90 +1758,90 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="75" t="e">
+      <c r="J6" s="67" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="76"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K6" s="68"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="70"/>
-      <c r="G7" s="70"/>
-      <c r="I7" s="71" t="s">
+      <c r="F7" s="76"/>
+      <c r="G7" s="76"/>
+      <c r="I7" s="77" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="71"/>
-      <c r="K7" s="71"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="69" t="e">
+      <c r="J7" s="77"/>
+      <c r="K7" s="77"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="75" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="69"/>
-      <c r="D8" s="69"/>
-      <c r="E8" s="69"/>
-      <c r="F8" s="69"/>
-      <c r="I8" s="72" t="s">
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="I8" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="72"/>
-      <c r="K8" s="72"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="73" t="e">
+      <c r="J8" s="78"/>
+      <c r="K8" s="78"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A9" s="79" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="I9" s="72" t="s">
+      <c r="B9" s="79"/>
+      <c r="C9" s="79"/>
+      <c r="D9" s="79"/>
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="I9" s="78" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="72"/>
-      <c r="K9" s="72"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="67" t="s">
+      <c r="J9" s="78"/>
+      <c r="K9" s="78"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="67" t="s">
+      <c r="B11" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="67" t="s">
+      <c r="C11" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="74" t="s">
+      <c r="D11" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74" t="s">
+      <c r="E11" s="80"/>
+      <c r="F11" s="80"/>
+      <c r="G11" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="74"/>
-      <c r="I11" s="74"/>
-      <c r="J11" s="67" t="s">
+      <c r="H11" s="80"/>
+      <c r="I11" s="80"/>
+      <c r="J11" s="73" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="68" t="s">
+      <c r="K11" s="74" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="67"/>
-      <c r="B12" s="67"/>
-      <c r="C12" s="67"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A12" s="73"/>
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -1426,10 +1860,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="67"/>
-      <c r="K12" s="68"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="J12" s="73"/>
+      <c r="K12" s="74"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="27" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1472,7 +1906,7 @@
       </c>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="27"/>
       <c r="B14" s="33" t="e">
         <f>#REF!</f>
@@ -1494,7 +1928,7 @@
       <c r="J14" s="28"/>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="12"/>
@@ -1507,7 +1941,7 @@
       <c r="J15" s="28"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16" s="27" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1550,7 +1984,7 @@
       </c>
       <c r="K16" s="14"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17" s="29"/>
       <c r="B17" s="29"/>
       <c r="C17" s="12"/>
@@ -1563,7 +1997,7 @@
       <c r="J17" s="28"/>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>16</v>
@@ -1589,13 +2023,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -1609,6 +2036,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1623,137 +2057,137 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S101"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="31.28515625" customWidth="1"/>
-    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.6640625" customWidth="1"/>
+    <col min="2" max="2" width="31.33203125" customWidth="1"/>
+    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="9.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.44140625" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" customWidth="1"/>
-    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.88671875" customWidth="1"/>
+    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="86" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="82" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
-      <c r="K1" s="86"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="87" t="s">
+      <c r="B1" s="82"/>
+      <c r="C1" s="82"/>
+      <c r="D1" s="82"/>
+      <c r="E1" s="82"/>
+      <c r="F1" s="82"/>
+      <c r="G1" s="82"/>
+      <c r="H1" s="82"/>
+      <c r="I1" s="82"/>
+      <c r="J1" s="82"/>
+      <c r="K1" s="82"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
+      <c r="A2" s="83" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="87"/>
-      <c r="C2" s="87"/>
-      <c r="D2" s="87"/>
-      <c r="E2" s="87"/>
-      <c r="F2" s="87"/>
-      <c r="G2" s="87"/>
-      <c r="H2" s="87"/>
-      <c r="I2" s="87"/>
-      <c r="J2" s="87"/>
-      <c r="K2" s="87"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="79" t="s">
+      <c r="B2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="71" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="79"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="79" t="s">
+      <c r="B3" s="71"/>
+      <c r="C3" s="71"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="71"/>
+      <c r="F3" s="71"/>
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="71" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="79"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-    </row>
-    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="88" t="s">
+      <c r="B4" s="71"/>
+      <c r="C4" s="71"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="71"/>
+      <c r="F4" s="71"/>
+      <c r="G4" s="71"/>
+      <c r="H4" s="71"/>
+      <c r="I4" s="71"/>
+      <c r="J4" s="71"/>
+      <c r="K4" s="71"/>
+    </row>
+    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A5" s="84" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="88"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="88"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="88"/>
-      <c r="G5" s="88"/>
-      <c r="H5" s="88"/>
-      <c r="I5" s="88"/>
-      <c r="J5" s="88"/>
-      <c r="K5" s="88"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="69" t="s">
+      <c r="B5" s="84"/>
+      <c r="C5" s="84"/>
+      <c r="D5" s="84"/>
+      <c r="E5" s="84"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="84"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="75" t="s">
         <v>46</v>
       </c>
-      <c r="B6" s="69"/>
-      <c r="C6" s="69"/>
-      <c r="D6" s="69"/>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="75"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="85" t="s">
+      <c r="H6" s="81" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="85"/>
-      <c r="J6" s="85"/>
-      <c r="K6" s="85"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="82" t="s">
+      <c r="I6" s="81"/>
+      <c r="J6" s="81"/>
+      <c r="K6" s="81"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="82"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="83" t="s">
+      <c r="H7" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="83"/>
-      <c r="J7" s="83"/>
-      <c r="K7" s="83"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I7" s="87"/>
+      <c r="J7" s="87"/>
+      <c r="K7" s="87"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -1788,7 +2222,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="1" customFormat="1" ht="54.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" s="1" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A9" s="63">
         <v>1</v>
       </c>
@@ -1805,7 +2239,7 @@
       <c r="J9" s="45"/>
       <c r="K9" s="29"/>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="18"/>
       <c r="B10" s="38" t="s">
         <v>48</v>
@@ -1829,7 +2263,9 @@
       <c r="H10" s="41"/>
       <c r="I10" s="41"/>
       <c r="J10" s="41"/>
-      <c r="K10" s="21"/>
+      <c r="K10" s="91" t="s">
+        <v>76</v>
+      </c>
       <c r="M10" s="25"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -1838,7 +2274,7 @@
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="18"/>
       <c r="B11" s="38" t="s">
         <v>49</v>
@@ -1862,7 +2298,7 @@
       <c r="H11" s="41"/>
       <c r="I11" s="41"/>
       <c r="J11" s="41"/>
-      <c r="K11" s="21"/>
+      <c r="K11" s="92"/>
       <c r="M11" s="25"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
@@ -1871,7 +2307,7 @@
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="18"/>
       <c r="B12" s="38" t="s">
         <v>50</v>
@@ -1893,7 +2329,7 @@
       <c r="H12" s="41"/>
       <c r="I12" s="41"/>
       <c r="J12" s="41"/>
-      <c r="K12" s="21"/>
+      <c r="K12" s="92"/>
       <c r="M12" s="25"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -1902,7 +2338,7 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="18"/>
       <c r="B13" s="38"/>
       <c r="C13" s="37">
@@ -1922,7 +2358,7 @@
       <c r="H13" s="41"/>
       <c r="I13" s="41"/>
       <c r="J13" s="41"/>
-      <c r="K13" s="21"/>
+      <c r="K13" s="92"/>
       <c r="M13" s="25"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -1931,7 +2367,7 @@
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
     </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="18"/>
       <c r="B14" s="38"/>
       <c r="C14" s="37">
@@ -1951,7 +2387,7 @@
       <c r="H14" s="41"/>
       <c r="I14" s="41"/>
       <c r="J14" s="41"/>
-      <c r="K14" s="21"/>
+      <c r="K14" s="93"/>
       <c r="M14" s="25"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -1960,7 +2396,7 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="18"/>
       <c r="B15" s="38" t="s">
         <v>41</v>
@@ -1992,7 +2428,7 @@
       <c r="R15" s="25"/>
       <c r="S15" s="25"/>
     </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="18"/>
       <c r="B16" s="38" t="s">
         <v>40</v>
@@ -2017,7 +2453,7 @@
       <c r="R16" s="25"/>
       <c r="S16" s="25"/>
     </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="18"/>
       <c r="B17" s="38"/>
       <c r="C17" s="37"/>
@@ -2037,12 +2473,12 @@
       <c r="R17" s="25"/>
       <c r="S17" s="25"/>
     </row>
-    <row r="18" spans="1:19" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" ht="55.2" x14ac:dyDescent="0.3">
       <c r="A18" s="18">
         <v>2</v>
       </c>
-      <c r="B18" s="65" t="s">
-        <v>51</v>
+      <c r="B18" s="89" t="s">
+        <v>67</v>
       </c>
       <c r="C18" s="37"/>
       <c r="D18" s="39"/>
@@ -2051,7 +2487,7 @@
       <c r="G18" s="40"/>
       <c r="H18" s="41"/>
       <c r="I18" s="41"/>
-      <c r="J18" s="45"/>
+      <c r="J18" s="41"/>
       <c r="K18" s="21"/>
       <c r="M18" s="25"/>
       <c r="N18" s="1"/>
@@ -2061,10 +2497,10 @@
       <c r="R18" s="25"/>
       <c r="S18" s="25"/>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="18"/>
       <c r="B19" s="38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="37">
         <v>1</v>
@@ -2088,7 +2524,7 @@
       <c r="R19" s="25"/>
       <c r="S19" s="25"/>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="18"/>
       <c r="B20" s="38" t="s">
         <v>41</v>
@@ -2120,7 +2556,7 @@
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
     </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="18"/>
       <c r="B21" s="38" t="s">
         <v>40</v>
@@ -2145,7 +2581,7 @@
       <c r="R21" s="25"/>
       <c r="S21" s="25"/>
     </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="18"/>
       <c r="B22" s="38"/>
       <c r="C22" s="37"/>
@@ -2165,30 +2601,34 @@
       <c r="R22" s="25"/>
       <c r="S22" s="25"/>
     </row>
-    <row r="23" spans="1:19" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" ht="28.2" x14ac:dyDescent="0.3">
       <c r="A23" s="18">
         <v>3</v>
       </c>
-      <c r="B23" s="66" t="s">
-        <v>53</v>
-      </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="40"/>
-      <c r="E23" s="40"/>
-      <c r="F23" s="40"/>
+      <c r="B23" s="65" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="37"/>
+      <c r="D23" s="39"/>
+      <c r="E23" s="39"/>
+      <c r="F23" s="39"/>
       <c r="G23" s="40"/>
-      <c r="H23" s="63"/>
-      <c r="I23" s="63"/>
+      <c r="H23" s="41"/>
+      <c r="I23" s="41"/>
       <c r="J23" s="45"/>
       <c r="K23" s="21"/>
-      <c r="M23" s="35"/>
-      <c r="R23" s="35"/>
-      <c r="S23" s="35"/>
-    </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M23" s="25"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="25"/>
+      <c r="S23" s="25"/>
+    </row>
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="18"/>
       <c r="B24" s="38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C24" s="37">
         <v>1</v>
@@ -2212,7 +2652,7 @@
       <c r="R24" s="25"/>
       <c r="S24" s="25"/>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="18"/>
       <c r="B25" s="38" t="s">
         <v>41</v>
@@ -2226,14 +2666,14 @@
         <v>1</v>
       </c>
       <c r="H25" s="41" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="I25" s="41">
-        <v>6062</v>
+        <v>1798</v>
       </c>
       <c r="J25" s="45">
         <f>G25*I25</f>
-        <v>6062</v>
+        <v>1798</v>
       </c>
       <c r="K25" s="21"/>
       <c r="M25" s="25"/>
@@ -2244,7 +2684,7 @@
       <c r="R25" s="25"/>
       <c r="S25" s="25"/>
     </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="18"/>
       <c r="B26" s="38" t="s">
         <v>40</v>
@@ -2258,7 +2698,7 @@
       <c r="I26" s="41"/>
       <c r="J26" s="45">
         <f>0.13*J25</f>
-        <v>788.06000000000006</v>
+        <v>233.74</v>
       </c>
       <c r="K26" s="21"/>
       <c r="M26" s="25"/>
@@ -2269,7 +2709,7 @@
       <c r="R26" s="25"/>
       <c r="S26" s="25"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="18"/>
       <c r="B27" s="38"/>
       <c r="C27" s="37"/>
@@ -2289,40 +2729,46 @@
       <c r="R27" s="25"/>
       <c r="S27" s="25"/>
     </row>
-    <row r="28" spans="1:19" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18">
         <v>4</v>
       </c>
-      <c r="B28" s="66" t="s">
-        <v>55</v>
-      </c>
-      <c r="C28" s="29"/>
-      <c r="D28" s="40"/>
-      <c r="E28" s="40"/>
-      <c r="F28" s="40"/>
+      <c r="B28" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="37"/>
+      <c r="D28" s="39"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
       <c r="G28" s="40"/>
-      <c r="H28" s="63"/>
-      <c r="I28" s="63"/>
+      <c r="H28" s="41"/>
+      <c r="I28" s="41"/>
       <c r="J28" s="45"/>
       <c r="K28" s="21"/>
-      <c r="M28" s="35"/>
-      <c r="R28" s="35"/>
-      <c r="S28" s="35"/>
-    </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M28" s="25"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="25"/>
+      <c r="S28" s="25"/>
+    </row>
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18"/>
       <c r="B29" s="38" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C29" s="37">
         <v>1</v>
       </c>
-      <c r="D29" s="39"/>
+      <c r="D29" s="39">
+        <v>2</v>
+      </c>
       <c r="E29" s="39"/>
       <c r="F29" s="39"/>
       <c r="G29" s="40">
         <f t="shared" ref="G29" si="3">PRODUCT(C29:F29)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H29" s="41"/>
       <c r="I29" s="41"/>
@@ -2336,7 +2782,7 @@
       <c r="R29" s="25"/>
       <c r="S29" s="25"/>
     </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18"/>
       <c r="B30" s="38" t="s">
         <v>41</v>
@@ -2347,17 +2793,18 @@
       <c r="F30" s="39"/>
       <c r="G30" s="34">
         <f>SUM(G29)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H30" s="41" t="s">
-        <v>43</v>
+        <v>56</v>
       </c>
       <c r="I30" s="41">
-        <v>1070</v>
+        <f>1230/40</f>
+        <v>30.75</v>
       </c>
       <c r="J30" s="45">
         <f>G30*I30</f>
-        <v>1070</v>
+        <v>61.5</v>
       </c>
       <c r="K30" s="21"/>
       <c r="M30" s="25"/>
@@ -2368,7 +2815,7 @@
       <c r="R30" s="25"/>
       <c r="S30" s="25"/>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="18"/>
       <c r="B31" s="38" t="s">
         <v>40</v>
@@ -2382,7 +2829,7 @@
       <c r="I31" s="41"/>
       <c r="J31" s="45">
         <f>0.13*J30</f>
-        <v>139.1</v>
+        <v>7.9950000000000001</v>
       </c>
       <c r="K31" s="21"/>
       <c r="M31" s="25"/>
@@ -2393,7 +2840,7 @@
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
     </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="18"/>
       <c r="B32" s="38"/>
       <c r="C32" s="37"/>
@@ -2413,81 +2860,75 @@
       <c r="R32" s="25"/>
       <c r="S32" s="25"/>
     </row>
-    <row r="33" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" s="1" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A33" s="18">
         <v>5</v>
       </c>
-      <c r="B33" s="30" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33" s="19">
+      <c r="B33" s="66" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="29"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="40"/>
+      <c r="F33" s="40"/>
+      <c r="G33" s="40"/>
+      <c r="H33" s="63"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="45"/>
+      <c r="K33" s="21"/>
+      <c r="M33" s="35"/>
+      <c r="R33" s="35"/>
+      <c r="S33" s="35"/>
+    </row>
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="18"/>
+      <c r="B34" s="38" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="37">
         <v>1</v>
       </c>
-      <c r="D33" s="20"/>
-      <c r="E33" s="21"/>
-      <c r="F33" s="21"/>
-      <c r="G33" s="34">
-        <f t="shared" ref="G33" si="4">PRODUCT(C33:F33)</f>
+      <c r="D34" s="39"/>
+      <c r="E34" s="39"/>
+      <c r="F34" s="39"/>
+      <c r="G34" s="40">
+        <f t="shared" ref="G34" si="4">PRODUCT(C34:F34)</f>
         <v>1</v>
       </c>
-      <c r="H33" s="22" t="s">
+      <c r="H34" s="41"/>
+      <c r="I34" s="41"/>
+      <c r="J34" s="45"/>
+      <c r="K34" s="21"/>
+      <c r="M34" s="25"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="25"/>
+      <c r="S34" s="25"/>
+    </row>
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="18"/>
+      <c r="B35" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="37"/>
+      <c r="D35" s="39"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
+      <c r="G35" s="34">
+        <f>SUM(G34)</f>
+        <v>1</v>
+      </c>
+      <c r="H35" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="I33" s="23">
-        <v>20000</v>
-      </c>
-      <c r="J33" s="34">
-        <f>G33*I33</f>
-        <v>20000</v>
-      </c>
-      <c r="K33" s="21"/>
-      <c r="M33" s="25"/>
-      <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
-      <c r="P33" s="1"/>
-      <c r="Q33" s="1"/>
-      <c r="R33" s="25"/>
-      <c r="S33" s="25"/>
-    </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="41"/>
-      <c r="B34" s="38"/>
-      <c r="C34" s="43"/>
-      <c r="D34" s="44"/>
-      <c r="E34" s="44"/>
-      <c r="F34" s="44"/>
-      <c r="G34" s="44"/>
-      <c r="H34" s="44"/>
-      <c r="I34" s="44"/>
-      <c r="J34" s="45"/>
-      <c r="K34" s="37"/>
-    </row>
-    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="18">
-        <v>5</v>
-      </c>
-      <c r="B35" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="C35" s="19">
-        <v>1</v>
-      </c>
-      <c r="D35" s="20"/>
-      <c r="E35" s="21"/>
-      <c r="F35" s="21"/>
-      <c r="G35" s="34">
-        <f t="shared" ref="G35" si="5">PRODUCT(C35:F35)</f>
-        <v>1</v>
-      </c>
-      <c r="H35" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="I35" s="23">
-        <v>500</v>
-      </c>
-      <c r="J35" s="34">
+      <c r="I35" s="41">
+        <v>5613</v>
+      </c>
+      <c r="J35" s="45">
         <f>G35*I35</f>
-        <v>500</v>
+        <v>5613</v>
       </c>
       <c r="K35" s="21"/>
       <c r="M35" s="25"/>
@@ -2498,17 +2939,22 @@
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
     </row>
-    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="18"/>
-      <c r="B36" s="24"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="21"/>
-      <c r="F36" s="21"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="22"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="42"/>
+      <c r="B36" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="37"/>
+      <c r="D36" s="39"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
+      <c r="G36" s="40"/>
+      <c r="H36" s="41"/>
+      <c r="I36" s="41"/>
+      <c r="J36" s="45">
+        <f>0.13*J35</f>
+        <v>729.69</v>
+      </c>
       <c r="K36" s="21"/>
       <c r="M36" s="25"/>
       <c r="N36" s="1"/>
@@ -2518,227 +2964,1381 @@
       <c r="R36" s="25"/>
       <c r="S36" s="25"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37" s="41"/>
-      <c r="B37" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="C37" s="47"/>
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="18"/>
+      <c r="B37" s="38"/>
+      <c r="C37" s="37"/>
       <c r="D37" s="39"/>
       <c r="E37" s="39"/>
       <c r="F37" s="39"/>
-      <c r="G37" s="42"/>
-      <c r="H37" s="42"/>
-      <c r="I37" s="42"/>
-      <c r="J37" s="42">
-        <f>SUM(J9:J35)</f>
-        <v>103926.71833909371</v>
-      </c>
-      <c r="K37" s="37"/>
-    </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38" s="58"/>
-      <c r="B38" s="61"/>
-      <c r="C38" s="62"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="60"/>
-      <c r="H38" s="60"/>
-      <c r="I38" s="60"/>
-      <c r="J38" s="60"/>
-      <c r="K38" s="57"/>
-    </row>
-    <row r="39" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="50"/>
-      <c r="B39" s="29" t="s">
+      <c r="G37" s="40"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="21"/>
+      <c r="M37" s="25"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="25"/>
+      <c r="S37" s="25"/>
+    </row>
+    <row r="38" spans="1:19" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="18">
+        <v>6</v>
+      </c>
+      <c r="B38" s="66" t="s">
+        <v>68</v>
+      </c>
+      <c r="C38" s="29"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="40"/>
+      <c r="G38" s="40"/>
+      <c r="H38" s="63"/>
+      <c r="I38" s="63"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="21"/>
+      <c r="M38" s="35"/>
+      <c r="R38" s="35"/>
+      <c r="S38" s="35"/>
+    </row>
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="18"/>
+      <c r="B39" s="38" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39" s="37">
+        <v>1</v>
+      </c>
+      <c r="D39" s="39"/>
+      <c r="E39" s="39"/>
+      <c r="F39" s="39"/>
+      <c r="G39" s="40">
+        <f t="shared" ref="G39" si="5">PRODUCT(C39:F39)</f>
+        <v>1</v>
+      </c>
+      <c r="H39" s="41"/>
+      <c r="I39" s="41"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="21"/>
+      <c r="M39" s="25"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="25"/>
+      <c r="S39" s="25"/>
+    </row>
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="18"/>
+      <c r="B40" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="37"/>
+      <c r="D40" s="39"/>
+      <c r="E40" s="39"/>
+      <c r="F40" s="39"/>
+      <c r="G40" s="34">
+        <f>SUM(G39)</f>
+        <v>1</v>
+      </c>
+      <c r="H40" s="41" t="s">
+        <v>43</v>
+      </c>
+      <c r="I40" s="41">
+        <v>1070</v>
+      </c>
+      <c r="J40" s="45">
+        <f>G40*I40</f>
+        <v>1070</v>
+      </c>
+      <c r="K40" s="21"/>
+      <c r="M40" s="25"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="25"/>
+      <c r="S40" s="25"/>
+    </row>
+    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="18"/>
+      <c r="B41" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C41" s="37"/>
+      <c r="D41" s="39"/>
+      <c r="E41" s="39"/>
+      <c r="F41" s="39"/>
+      <c r="G41" s="40"/>
+      <c r="H41" s="41"/>
+      <c r="I41" s="41"/>
+      <c r="J41" s="45">
+        <f>0.13*J40</f>
+        <v>139.1</v>
+      </c>
+      <c r="K41" s="21"/>
+      <c r="M41" s="25"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="25"/>
+      <c r="S41" s="25"/>
+    </row>
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="18"/>
+      <c r="B42" s="38"/>
+      <c r="C42" s="37"/>
+      <c r="D42" s="39"/>
+      <c r="E42" s="39"/>
+      <c r="F42" s="39"/>
+      <c r="G42" s="40"/>
+      <c r="H42" s="41"/>
+      <c r="I42" s="41"/>
+      <c r="J42" s="45"/>
+      <c r="K42" s="21"/>
+      <c r="M42" s="25"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="25"/>
+      <c r="S42" s="25"/>
+    </row>
+    <row r="43" spans="1:19" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A43" s="18">
+        <v>7</v>
+      </c>
+      <c r="B43" s="90" t="s">
+        <v>69</v>
+      </c>
+      <c r="C43" s="37"/>
+      <c r="D43" s="39"/>
+      <c r="E43" s="39"/>
+      <c r="F43" s="39"/>
+      <c r="G43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="45"/>
+      <c r="K43" s="21"/>
+      <c r="M43" s="25"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="25"/>
+      <c r="S43" s="25"/>
+    </row>
+    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="18"/>
+      <c r="B44" s="38" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="37">
+        <v>1</v>
+      </c>
+      <c r="D44" s="39"/>
+      <c r="E44" s="39"/>
+      <c r="F44" s="39"/>
+      <c r="G44" s="40">
+        <f t="shared" ref="G44" si="6">PRODUCT(C44:F44)</f>
+        <v>1</v>
+      </c>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="45"/>
+      <c r="K44" s="21"/>
+      <c r="M44" s="25"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="25"/>
+      <c r="S44" s="25"/>
+    </row>
+    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="18"/>
+      <c r="B45" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C45" s="37"/>
+      <c r="D45" s="39"/>
+      <c r="E45" s="39"/>
+      <c r="F45" s="39"/>
+      <c r="G45" s="34">
+        <f>SUM(G44)</f>
+        <v>1</v>
+      </c>
+      <c r="H45" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="I45" s="41">
+        <v>4425</v>
+      </c>
+      <c r="J45" s="45">
+        <f>G45*I45</f>
+        <v>4425</v>
+      </c>
+      <c r="K45" s="21"/>
+      <c r="M45" s="25"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="25"/>
+      <c r="S45" s="25"/>
+    </row>
+    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="18"/>
+      <c r="B46" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C46" s="37"/>
+      <c r="D46" s="39"/>
+      <c r="E46" s="39"/>
+      <c r="F46" s="39"/>
+      <c r="G46" s="40"/>
+      <c r="H46" s="41"/>
+      <c r="I46" s="41"/>
+      <c r="J46" s="45">
+        <f>0.13*J45</f>
+        <v>575.25</v>
+      </c>
+      <c r="K46" s="21"/>
+      <c r="M46" s="25"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="25"/>
+      <c r="S46" s="25"/>
+    </row>
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="18"/>
+      <c r="B47" s="38"/>
+      <c r="C47" s="37"/>
+      <c r="D47" s="39"/>
+      <c r="E47" s="39"/>
+      <c r="F47" s="39"/>
+      <c r="G47" s="40"/>
+      <c r="H47" s="41"/>
+      <c r="I47" s="41"/>
+      <c r="J47" s="45"/>
+      <c r="K47" s="21"/>
+      <c r="M47" s="25"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="25"/>
+      <c r="S47" s="25"/>
+    </row>
+    <row r="48" spans="1:19" ht="42" x14ac:dyDescent="0.3">
+      <c r="A48" s="18">
+        <v>8</v>
+      </c>
+      <c r="B48" s="90" t="s">
+        <v>70</v>
+      </c>
+      <c r="C48" s="37"/>
+      <c r="D48" s="39"/>
+      <c r="E48" s="39"/>
+      <c r="F48" s="39"/>
+      <c r="G48" s="40"/>
+      <c r="H48" s="41"/>
+      <c r="I48" s="41"/>
+      <c r="J48" s="45"/>
+      <c r="K48" s="21"/>
+      <c r="M48" s="25"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="25"/>
+      <c r="S48" s="25"/>
+    </row>
+    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A49" s="18"/>
+      <c r="B49" s="38" t="s">
+        <v>60</v>
+      </c>
+      <c r="C49" s="37">
+        <v>1</v>
+      </c>
+      <c r="D49" s="39"/>
+      <c r="E49" s="39"/>
+      <c r="F49" s="39"/>
+      <c r="G49" s="40">
+        <f t="shared" ref="G49" si="7">PRODUCT(C49:F49)</f>
+        <v>1</v>
+      </c>
+      <c r="H49" s="41"/>
+      <c r="I49" s="41"/>
+      <c r="J49" s="45"/>
+      <c r="K49" s="21"/>
+      <c r="M49" s="25"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="25"/>
+      <c r="S49" s="25"/>
+    </row>
+    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="18"/>
+      <c r="B50" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C50" s="37"/>
+      <c r="D50" s="39"/>
+      <c r="E50" s="39"/>
+      <c r="F50" s="39"/>
+      <c r="G50" s="34">
+        <f>SUM(G49)</f>
+        <v>1</v>
+      </c>
+      <c r="H50" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="I50" s="41">
+        <v>1459</v>
+      </c>
+      <c r="J50" s="45">
+        <f>G50*I50</f>
+        <v>1459</v>
+      </c>
+      <c r="K50" s="21"/>
+      <c r="M50" s="25"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="1"/>
+      <c r="R50" s="25"/>
+      <c r="S50" s="25"/>
+    </row>
+    <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="18"/>
+      <c r="B51" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" s="37"/>
+      <c r="D51" s="39"/>
+      <c r="E51" s="39"/>
+      <c r="F51" s="39"/>
+      <c r="G51" s="40"/>
+      <c r="H51" s="41"/>
+      <c r="I51" s="41"/>
+      <c r="J51" s="45">
+        <f>0.13*J50</f>
+        <v>189.67000000000002</v>
+      </c>
+      <c r="K51" s="21"/>
+      <c r="M51" s="25"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="25"/>
+      <c r="S51" s="25"/>
+    </row>
+    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A52" s="18"/>
+      <c r="B52" s="38"/>
+      <c r="C52" s="37"/>
+      <c r="D52" s="39"/>
+      <c r="E52" s="39"/>
+      <c r="F52" s="39"/>
+      <c r="G52" s="40"/>
+      <c r="H52" s="41"/>
+      <c r="I52" s="41"/>
+      <c r="J52" s="45"/>
+      <c r="K52" s="21"/>
+      <c r="M52" s="25"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="25"/>
+      <c r="S52" s="25"/>
+    </row>
+    <row r="53" spans="1:19" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A53" s="18">
+        <v>9</v>
+      </c>
+      <c r="B53" s="90" t="s">
+        <v>71</v>
+      </c>
+      <c r="C53" s="37"/>
+      <c r="D53" s="39"/>
+      <c r="E53" s="39"/>
+      <c r="F53" s="39"/>
+      <c r="G53" s="40"/>
+      <c r="H53" s="41"/>
+      <c r="I53" s="41"/>
+      <c r="J53" s="45"/>
+      <c r="K53" s="21"/>
+      <c r="M53" s="25"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="25"/>
+      <c r="S53" s="25"/>
+    </row>
+    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="18"/>
+      <c r="B54" s="38" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54" s="37">
+        <v>1</v>
+      </c>
+      <c r="D54" s="39"/>
+      <c r="E54" s="39"/>
+      <c r="F54" s="39"/>
+      <c r="G54" s="40">
+        <f t="shared" ref="G54" si="8">PRODUCT(C54:F54)</f>
+        <v>1</v>
+      </c>
+      <c r="H54" s="41"/>
+      <c r="I54" s="41"/>
+      <c r="J54" s="45"/>
+      <c r="K54" s="21"/>
+      <c r="M54" s="25"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="25"/>
+      <c r="S54" s="25"/>
+    </row>
+    <row r="55" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="18"/>
+      <c r="B55" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C55" s="37"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="34">
+        <f>SUM(G54)</f>
+        <v>1</v>
+      </c>
+      <c r="H55" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="I55" s="41">
+        <v>4182</v>
+      </c>
+      <c r="J55" s="45">
+        <f>G55*I55</f>
+        <v>4182</v>
+      </c>
+      <c r="K55" s="21"/>
+      <c r="M55" s="25"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="25"/>
+      <c r="S55" s="25"/>
+    </row>
+    <row r="56" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="18"/>
+      <c r="B56" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C56" s="37"/>
+      <c r="D56" s="39"/>
+      <c r="E56" s="39"/>
+      <c r="F56" s="39"/>
+      <c r="G56" s="40"/>
+      <c r="H56" s="41"/>
+      <c r="I56" s="41"/>
+      <c r="J56" s="45">
+        <f>0.13*J55</f>
+        <v>543.66</v>
+      </c>
+      <c r="K56" s="21"/>
+      <c r="M56" s="25"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="25"/>
+      <c r="S56" s="25"/>
+    </row>
+    <row r="57" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="18"/>
+      <c r="B57" s="38"/>
+      <c r="C57" s="37"/>
+      <c r="D57" s="39"/>
+      <c r="E57" s="39"/>
+      <c r="F57" s="39"/>
+      <c r="G57" s="40"/>
+      <c r="H57" s="41"/>
+      <c r="I57" s="41"/>
+      <c r="J57" s="45"/>
+      <c r="K57" s="21"/>
+      <c r="M57" s="25"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="25"/>
+      <c r="S57" s="25"/>
+    </row>
+    <row r="58" spans="1:19" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A58" s="18">
+        <v>10</v>
+      </c>
+      <c r="B58" s="90" t="s">
+        <v>72</v>
+      </c>
+      <c r="C58" s="37"/>
+      <c r="D58" s="39"/>
+      <c r="E58" s="39"/>
+      <c r="F58" s="39"/>
+      <c r="G58" s="40"/>
+      <c r="H58" s="41"/>
+      <c r="I58" s="41"/>
+      <c r="J58" s="45"/>
+      <c r="K58" s="21"/>
+      <c r="M58" s="25"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="25"/>
+      <c r="S58" s="25"/>
+    </row>
+    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="18"/>
+      <c r="B59" s="38" t="s">
+        <v>62</v>
+      </c>
+      <c r="C59" s="37">
+        <v>1</v>
+      </c>
+      <c r="D59" s="39"/>
+      <c r="E59" s="39"/>
+      <c r="F59" s="39"/>
+      <c r="G59" s="40">
+        <f t="shared" ref="G59" si="9">PRODUCT(C59:F59)</f>
+        <v>1</v>
+      </c>
+      <c r="H59" s="41"/>
+      <c r="I59" s="41"/>
+      <c r="J59" s="45"/>
+      <c r="K59" s="21"/>
+      <c r="M59" s="25"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="25"/>
+      <c r="S59" s="25"/>
+    </row>
+    <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="18"/>
+      <c r="B60" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C60" s="37"/>
+      <c r="D60" s="39"/>
+      <c r="E60" s="39"/>
+      <c r="F60" s="39"/>
+      <c r="G60" s="34">
+        <f>SUM(G59)</f>
+        <v>1</v>
+      </c>
+      <c r="H60" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="I60" s="41">
+        <v>5565</v>
+      </c>
+      <c r="J60" s="45">
+        <f>G60*I60</f>
+        <v>5565</v>
+      </c>
+      <c r="K60" s="21"/>
+      <c r="M60" s="25"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="25"/>
+      <c r="S60" s="25"/>
+    </row>
+    <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="18"/>
+      <c r="B61" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C61" s="37"/>
+      <c r="D61" s="39"/>
+      <c r="E61" s="39"/>
+      <c r="F61" s="39"/>
+      <c r="G61" s="40"/>
+      <c r="H61" s="41"/>
+      <c r="I61" s="41"/>
+      <c r="J61" s="45">
+        <f>0.13*J60</f>
+        <v>723.45</v>
+      </c>
+      <c r="K61" s="21"/>
+      <c r="M61" s="25"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="25"/>
+      <c r="S61" s="25"/>
+    </row>
+    <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="18"/>
+      <c r="B62" s="38"/>
+      <c r="C62" s="37"/>
+      <c r="D62" s="39"/>
+      <c r="E62" s="39"/>
+      <c r="F62" s="39"/>
+      <c r="G62" s="40"/>
+      <c r="H62" s="41"/>
+      <c r="I62" s="41"/>
+      <c r="J62" s="45"/>
+      <c r="K62" s="21"/>
+      <c r="M62" s="25"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="25"/>
+      <c r="S62" s="25"/>
+    </row>
+    <row r="63" spans="1:19" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A63" s="18">
+        <v>11</v>
+      </c>
+      <c r="B63" s="90" t="s">
+        <v>73</v>
+      </c>
+      <c r="C63" s="37"/>
+      <c r="D63" s="39"/>
+      <c r="E63" s="39"/>
+      <c r="F63" s="39"/>
+      <c r="G63" s="40"/>
+      <c r="H63" s="41"/>
+      <c r="I63" s="41"/>
+      <c r="J63" s="45"/>
+      <c r="K63" s="21"/>
+      <c r="M63" s="25"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="25"/>
+      <c r="S63" s="25"/>
+    </row>
+    <row r="64" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="18"/>
+      <c r="B64" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C64" s="37">
+        <v>1</v>
+      </c>
+      <c r="D64" s="39"/>
+      <c r="E64" s="39"/>
+      <c r="F64" s="39"/>
+      <c r="G64" s="40">
+        <f t="shared" ref="G64" si="10">PRODUCT(C64:F64)</f>
+        <v>1</v>
+      </c>
+      <c r="H64" s="41"/>
+      <c r="I64" s="41"/>
+      <c r="J64" s="45"/>
+      <c r="K64" s="21"/>
+      <c r="M64" s="25"/>
+      <c r="N64" s="1"/>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="25"/>
+      <c r="S64" s="25"/>
+    </row>
+    <row r="65" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="18"/>
+      <c r="B65" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C65" s="37"/>
+      <c r="D65" s="39"/>
+      <c r="E65" s="39"/>
+      <c r="F65" s="39"/>
+      <c r="G65" s="34">
+        <f>SUM(G64)</f>
+        <v>1</v>
+      </c>
+      <c r="H65" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="I65" s="41">
+        <v>929</v>
+      </c>
+      <c r="J65" s="45">
+        <f>G65*I65</f>
+        <v>929</v>
+      </c>
+      <c r="K65" s="21"/>
+      <c r="M65" s="25"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="25"/>
+      <c r="S65" s="25"/>
+    </row>
+    <row r="66" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="18"/>
+      <c r="B66" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C66" s="37"/>
+      <c r="D66" s="39"/>
+      <c r="E66" s="39"/>
+      <c r="F66" s="39"/>
+      <c r="G66" s="40"/>
+      <c r="H66" s="41"/>
+      <c r="I66" s="41"/>
+      <c r="J66" s="45">
+        <f>0.13*J65</f>
+        <v>120.77000000000001</v>
+      </c>
+      <c r="K66" s="21"/>
+      <c r="M66" s="25"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="25"/>
+      <c r="S66" s="25"/>
+    </row>
+    <row r="67" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="18"/>
+      <c r="B67" s="38"/>
+      <c r="C67" s="37"/>
+      <c r="D67" s="39"/>
+      <c r="E67" s="39"/>
+      <c r="F67" s="39"/>
+      <c r="G67" s="40"/>
+      <c r="H67" s="41"/>
+      <c r="I67" s="41"/>
+      <c r="J67" s="45"/>
+      <c r="K67" s="21"/>
+      <c r="M67" s="25"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="25"/>
+      <c r="S67" s="25"/>
+    </row>
+    <row r="68" spans="1:19" ht="28.2" x14ac:dyDescent="0.3">
+      <c r="A68" s="18">
+        <v>12</v>
+      </c>
+      <c r="B68" s="90" t="s">
+        <v>74</v>
+      </c>
+      <c r="C68" s="37"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="40"/>
+      <c r="H68" s="41"/>
+      <c r="I68" s="41"/>
+      <c r="J68" s="45"/>
+      <c r="K68" s="21"/>
+      <c r="M68" s="25"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="25"/>
+      <c r="S68" s="25"/>
+    </row>
+    <row r="69" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="18"/>
+      <c r="B69" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C69" s="37">
+        <v>1</v>
+      </c>
+      <c r="D69" s="39"/>
+      <c r="E69" s="39"/>
+      <c r="F69" s="39"/>
+      <c r="G69" s="40">
+        <f t="shared" ref="G69" si="11">PRODUCT(C69:F69)</f>
+        <v>1</v>
+      </c>
+      <c r="H69" s="41"/>
+      <c r="I69" s="41"/>
+      <c r="J69" s="45"/>
+      <c r="K69" s="21"/>
+      <c r="M69" s="25"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="25"/>
+      <c r="S69" s="25"/>
+    </row>
+    <row r="70" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="18"/>
+      <c r="B70" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C70" s="37"/>
+      <c r="D70" s="39"/>
+      <c r="E70" s="39"/>
+      <c r="F70" s="39"/>
+      <c r="G70" s="34">
+        <f>SUM(G69)</f>
+        <v>1</v>
+      </c>
+      <c r="H70" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="I70" s="41">
+        <v>510</v>
+      </c>
+      <c r="J70" s="45">
+        <f>G70*I70</f>
+        <v>510</v>
+      </c>
+      <c r="K70" s="21"/>
+      <c r="M70" s="25"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="25"/>
+      <c r="S70" s="25"/>
+    </row>
+    <row r="71" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A71" s="18"/>
+      <c r="B71" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C71" s="37"/>
+      <c r="D71" s="39"/>
+      <c r="E71" s="39"/>
+      <c r="F71" s="39"/>
+      <c r="G71" s="40"/>
+      <c r="H71" s="41"/>
+      <c r="I71" s="41"/>
+      <c r="J71" s="45">
+        <f>0.13*J70</f>
+        <v>66.3</v>
+      </c>
+      <c r="K71" s="21"/>
+      <c r="M71" s="25"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="25"/>
+      <c r="S71" s="25"/>
+    </row>
+    <row r="72" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="18"/>
+      <c r="B72" s="38"/>
+      <c r="C72" s="37"/>
+      <c r="D72" s="39"/>
+      <c r="E72" s="39"/>
+      <c r="F72" s="39"/>
+      <c r="G72" s="40"/>
+      <c r="H72" s="41"/>
+      <c r="I72" s="41"/>
+      <c r="J72" s="45"/>
+      <c r="K72" s="21"/>
+      <c r="M72" s="25"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="25"/>
+      <c r="S72" s="25"/>
+    </row>
+    <row r="73" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="18">
+        <v>13</v>
+      </c>
+      <c r="B73" s="90" t="s">
+        <v>75</v>
+      </c>
+      <c r="C73" s="37"/>
+      <c r="D73" s="39"/>
+      <c r="E73" s="39"/>
+      <c r="F73" s="39"/>
+      <c r="G73" s="40"/>
+      <c r="H73" s="41"/>
+      <c r="I73" s="41"/>
+      <c r="J73" s="45"/>
+      <c r="K73" s="21"/>
+      <c r="M73" s="25"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="25"/>
+      <c r="S73" s="25"/>
+    </row>
+    <row r="74" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="18"/>
+      <c r="B74" s="38" t="s">
+        <v>63</v>
+      </c>
+      <c r="C74" s="37">
+        <v>1</v>
+      </c>
+      <c r="D74" s="39"/>
+      <c r="E74" s="39"/>
+      <c r="F74" s="39"/>
+      <c r="G74" s="40">
+        <f t="shared" ref="G74" si="12">PRODUCT(C74:F74)</f>
+        <v>1</v>
+      </c>
+      <c r="H74" s="41"/>
+      <c r="I74" s="41"/>
+      <c r="J74" s="45"/>
+      <c r="K74" s="21"/>
+      <c r="M74" s="25"/>
+      <c r="N74" s="1"/>
+      <c r="O74" s="1"/>
+      <c r="P74" s="1"/>
+      <c r="Q74" s="1"/>
+      <c r="R74" s="25"/>
+      <c r="S74" s="25"/>
+    </row>
+    <row r="75" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="18"/>
+      <c r="B75" s="38" t="s">
+        <v>41</v>
+      </c>
+      <c r="C75" s="37"/>
+      <c r="D75" s="39"/>
+      <c r="E75" s="39"/>
+      <c r="F75" s="39"/>
+      <c r="G75" s="34">
+        <f>SUM(G74)</f>
+        <v>1</v>
+      </c>
+      <c r="H75" s="41" t="s">
+        <v>31</v>
+      </c>
+      <c r="I75" s="41">
+        <v>680</v>
+      </c>
+      <c r="J75" s="45">
+        <f>G75*I75</f>
+        <v>680</v>
+      </c>
+      <c r="K75" s="21"/>
+      <c r="M75" s="25"/>
+      <c r="N75" s="1"/>
+      <c r="O75" s="1"/>
+      <c r="P75" s="1"/>
+      <c r="Q75" s="1"/>
+      <c r="R75" s="25"/>
+      <c r="S75" s="25"/>
+    </row>
+    <row r="76" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A76" s="18"/>
+      <c r="B76" s="38" t="s">
+        <v>40</v>
+      </c>
+      <c r="C76" s="37"/>
+      <c r="D76" s="39"/>
+      <c r="E76" s="39"/>
+      <c r="F76" s="39"/>
+      <c r="G76" s="40"/>
+      <c r="H76" s="41"/>
+      <c r="I76" s="41"/>
+      <c r="J76" s="45">
+        <f>0.13*J75</f>
+        <v>88.4</v>
+      </c>
+      <c r="K76" s="21"/>
+      <c r="M76" s="25"/>
+      <c r="N76" s="1"/>
+      <c r="O76" s="1"/>
+      <c r="P76" s="1"/>
+      <c r="Q76" s="1"/>
+      <c r="R76" s="25"/>
+      <c r="S76" s="25"/>
+    </row>
+    <row r="77" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="18"/>
+      <c r="B77" s="38"/>
+      <c r="C77" s="37"/>
+      <c r="D77" s="39"/>
+      <c r="E77" s="39"/>
+      <c r="F77" s="39"/>
+      <c r="G77" s="40"/>
+      <c r="H77" s="41"/>
+      <c r="I77" s="41"/>
+      <c r="J77" s="45"/>
+      <c r="K77" s="21"/>
+      <c r="M77" s="25"/>
+      <c r="N77" s="1"/>
+      <c r="O77" s="1"/>
+      <c r="P77" s="1"/>
+      <c r="Q77" s="1"/>
+      <c r="R77" s="25"/>
+      <c r="S77" s="25"/>
+    </row>
+    <row r="78" spans="1:19" ht="19.8" x14ac:dyDescent="0.3">
+      <c r="A78" s="18">
+        <v>14</v>
+      </c>
+      <c r="B78" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="C78" s="19">
+        <v>1</v>
+      </c>
+      <c r="D78" s="20"/>
+      <c r="E78" s="21"/>
+      <c r="F78" s="21"/>
+      <c r="G78" s="34">
+        <f t="shared" ref="G78" si="13">PRODUCT(C78:F78)</f>
+        <v>1</v>
+      </c>
+      <c r="H78" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I78" s="23">
+        <v>12000</v>
+      </c>
+      <c r="J78" s="34">
+        <f>G78*I78</f>
+        <v>12000</v>
+      </c>
+      <c r="K78" s="21"/>
+      <c r="M78" s="25"/>
+      <c r="N78" s="1"/>
+      <c r="O78" s="1"/>
+      <c r="P78" s="1"/>
+      <c r="Q78" s="1"/>
+      <c r="R78" s="25"/>
+      <c r="S78" s="25"/>
+    </row>
+    <row r="79" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A79" s="41"/>
+      <c r="B79" s="38"/>
+      <c r="C79" s="43"/>
+      <c r="D79" s="44"/>
+      <c r="E79" s="44"/>
+      <c r="F79" s="44"/>
+      <c r="G79" s="44"/>
+      <c r="H79" s="44"/>
+      <c r="I79" s="44"/>
+      <c r="J79" s="45"/>
+      <c r="K79" s="37"/>
+    </row>
+    <row r="80" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A80" s="18">
+        <v>15</v>
+      </c>
+      <c r="B80" s="30" t="s">
+        <v>30</v>
+      </c>
+      <c r="C80" s="19">
+        <v>1</v>
+      </c>
+      <c r="D80" s="20"/>
+      <c r="E80" s="21"/>
+      <c r="F80" s="21"/>
+      <c r="G80" s="34">
+        <f t="shared" ref="G80" si="14">PRODUCT(C80:F80)</f>
+        <v>1</v>
+      </c>
+      <c r="H80" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="I80" s="23">
+        <v>500</v>
+      </c>
+      <c r="J80" s="34">
+        <f>G80*I80</f>
+        <v>500</v>
+      </c>
+      <c r="K80" s="21"/>
+      <c r="M80" s="25"/>
+      <c r="N80" s="1"/>
+      <c r="O80" s="1"/>
+      <c r="P80" s="1"/>
+      <c r="Q80" s="1"/>
+      <c r="R80" s="25"/>
+      <c r="S80" s="25"/>
+    </row>
+    <row r="81" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="18"/>
+      <c r="B81" s="24"/>
+      <c r="C81" s="19"/>
+      <c r="D81" s="20"/>
+      <c r="E81" s="21"/>
+      <c r="F81" s="21"/>
+      <c r="G81" s="23"/>
+      <c r="H81" s="22"/>
+      <c r="I81" s="23"/>
+      <c r="J81" s="42"/>
+      <c r="K81" s="21"/>
+      <c r="M81" s="25"/>
+      <c r="N81" s="1"/>
+      <c r="O81" s="1"/>
+      <c r="P81" s="1"/>
+      <c r="Q81" s="1"/>
+      <c r="R81" s="25"/>
+      <c r="S81" s="25"/>
+    </row>
+    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A82" s="41"/>
+      <c r="B82" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C82" s="47"/>
+      <c r="D82" s="39"/>
+      <c r="E82" s="39"/>
+      <c r="F82" s="39"/>
+      <c r="G82" s="42"/>
+      <c r="H82" s="42"/>
+      <c r="I82" s="42"/>
+      <c r="J82" s="42">
+        <f>SUM(J9:J80)</f>
+        <v>117578.08333909372</v>
+      </c>
+      <c r="K82" s="37"/>
+    </row>
+    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A83" s="58"/>
+      <c r="B83" s="61"/>
+      <c r="C83" s="62"/>
+      <c r="D83" s="59"/>
+      <c r="E83" s="59"/>
+      <c r="F83" s="59"/>
+      <c r="G83" s="60"/>
+      <c r="H83" s="60"/>
+      <c r="I83" s="60"/>
+      <c r="J83" s="60"/>
+      <c r="K83" s="57"/>
+    </row>
+    <row r="84" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A84" s="50"/>
+      <c r="B84" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C39" s="81">
-        <f>J37</f>
-        <v>103926.71833909371</v>
-      </c>
-      <c r="D39" s="81"/>
-      <c r="E39" s="40">
+      <c r="C84" s="85">
+        <f>J82</f>
+        <v>117578.08333909372</v>
+      </c>
+      <c r="D84" s="85"/>
+      <c r="E84" s="40">
         <v>100</v>
       </c>
-      <c r="F39" s="51"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="51"/>
-      <c r="I39" s="53"/>
-      <c r="J39" s="54"/>
-      <c r="K39" s="55"/>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40" s="56"/>
-      <c r="B40" s="29" t="s">
+      <c r="F84" s="51"/>
+      <c r="G84" s="52"/>
+      <c r="H84" s="51"/>
+      <c r="I84" s="53"/>
+      <c r="J84" s="54"/>
+      <c r="K84" s="55"/>
+    </row>
+    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A85" s="56"/>
+      <c r="B85" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C40" s="84">
+      <c r="C85" s="88">
         <v>100000</v>
       </c>
-      <c r="D40" s="84"/>
-      <c r="E40" s="40"/>
-      <c r="F40" s="49"/>
-      <c r="G40" s="48"/>
-      <c r="H40" s="48"/>
-      <c r="I40" s="48"/>
-      <c r="J40" s="48"/>
-      <c r="K40" s="49"/>
-    </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41" s="56"/>
-      <c r="B41" s="29" t="s">
+      <c r="D85" s="88"/>
+      <c r="E85" s="40"/>
+      <c r="F85" s="49"/>
+      <c r="G85" s="48"/>
+      <c r="H85" s="48"/>
+      <c r="I85" s="48"/>
+      <c r="J85" s="48"/>
+      <c r="K85" s="49"/>
+    </row>
+    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A86" s="56"/>
+      <c r="B86" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C41" s="84">
-        <f>C40-C43-C44</f>
+      <c r="C86" s="88">
+        <f>C85-C88-C89</f>
         <v>95000</v>
       </c>
-      <c r="D41" s="84"/>
-      <c r="E41" s="40">
-        <f>C41/C39*100</f>
-        <v>91.410564596134478</v>
-      </c>
-      <c r="F41" s="49"/>
-      <c r="G41" s="48"/>
-      <c r="H41" s="48"/>
-      <c r="I41" s="48"/>
-      <c r="J41" s="48"/>
-      <c r="K41" s="49"/>
-    </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42" s="56"/>
-      <c r="B42" s="29" t="s">
+      <c r="D86" s="88"/>
+      <c r="E86" s="40">
+        <f>C86/C84*100</f>
+        <v>80.797370821244968</v>
+      </c>
+      <c r="F86" s="49"/>
+      <c r="G86" s="48"/>
+      <c r="H86" s="48"/>
+      <c r="I86" s="48"/>
+      <c r="J86" s="48"/>
+      <c r="K86" s="49"/>
+    </row>
+    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A87" s="56"/>
+      <c r="B87" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C42" s="81">
-        <f>C39-C41</f>
-        <v>8926.7183390937134</v>
-      </c>
-      <c r="D42" s="81"/>
-      <c r="E42" s="40">
-        <f>100-E41</f>
-        <v>8.5894354038655223</v>
-      </c>
-      <c r="F42" s="49"/>
-      <c r="G42" s="48"/>
-      <c r="H42" s="48"/>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
-      <c r="K42" s="49"/>
-    </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A43" s="56"/>
-      <c r="B43" s="29" t="s">
+      <c r="C87" s="85">
+        <f>C84-C86</f>
+        <v>22578.083339093719</v>
+      </c>
+      <c r="D87" s="85"/>
+      <c r="E87" s="40">
+        <f>100-E86</f>
+        <v>19.202629178755032</v>
+      </c>
+      <c r="F87" s="49"/>
+      <c r="G87" s="48"/>
+      <c r="H87" s="48"/>
+      <c r="I87" s="48"/>
+      <c r="J87" s="48"/>
+      <c r="K87" s="49"/>
+    </row>
+    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A88" s="56"/>
+      <c r="B88" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C43" s="81">
-        <f>C40*0.03</f>
+      <c r="C88" s="85">
+        <f>C85*0.03</f>
         <v>3000</v>
       </c>
-      <c r="D43" s="81"/>
-      <c r="E43" s="40">
+      <c r="D88" s="85"/>
+      <c r="E88" s="40">
         <v>3</v>
       </c>
-      <c r="F43" s="49"/>
-      <c r="G43" s="48"/>
-      <c r="H43" s="48"/>
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
-      <c r="K43" s="49"/>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A44" s="56"/>
-      <c r="B44" s="29" t="s">
+      <c r="F88" s="49"/>
+      <c r="G88" s="48"/>
+      <c r="H88" s="48"/>
+      <c r="I88" s="48"/>
+      <c r="J88" s="48"/>
+      <c r="K88" s="49"/>
+    </row>
+    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A89" s="56"/>
+      <c r="B89" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C44" s="81">
-        <f>C40*0.02</f>
+      <c r="C89" s="85">
+        <f>C85*0.02</f>
         <v>2000</v>
       </c>
-      <c r="D44" s="81"/>
-      <c r="E44" s="40">
+      <c r="D89" s="85"/>
+      <c r="E89" s="40">
         <v>2</v>
       </c>
-      <c r="F44" s="49"/>
-      <c r="G44" s="48"/>
-      <c r="H44" s="48"/>
-      <c r="I44" s="48"/>
-      <c r="J44" s="48"/>
-      <c r="K44" s="49"/>
-    </row>
-    <row r="45" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="57"/>
-      <c r="B45" s="57"/>
-      <c r="C45" s="57"/>
-      <c r="D45" s="57"/>
-      <c r="E45" s="57"/>
-      <c r="F45" s="57"/>
-      <c r="G45" s="57"/>
-      <c r="H45" s="57"/>
-      <c r="I45" s="57"/>
-      <c r="J45" s="57"/>
-      <c r="K45" s="57"/>
-    </row>
-    <row r="46" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="59" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="60" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="61" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="62" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="63" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="64" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="65" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="66" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="67" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="68" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="69" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="70" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="71" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="72" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="73" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="74" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="75" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="76" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="77" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="78" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="79" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="80" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="81" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="82" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="83" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="84" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="85" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="86" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="87" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="88" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="89" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="90" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="91" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="92" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="93" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="94" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="95" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="96" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="97" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="98" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="99" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="100" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="101" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+      <c r="F89" s="49"/>
+      <c r="G89" s="48"/>
+      <c r="H89" s="48"/>
+      <c r="I89" s="48"/>
+      <c r="J89" s="48"/>
+      <c r="K89" s="49"/>
+    </row>
+    <row r="90" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A90" s="57"/>
+      <c r="B90" s="57"/>
+      <c r="C90" s="57"/>
+      <c r="D90" s="57"/>
+      <c r="E90" s="57"/>
+      <c r="F90" s="57"/>
+      <c r="G90" s="57"/>
+      <c r="H90" s="57"/>
+      <c r="I90" s="57"/>
+      <c r="J90" s="57"/>
+      <c r="K90" s="57"/>
+    </row>
+    <row r="91" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="95" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="96" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="97" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="98" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="99" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="100" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="101" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="102" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="103" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="104" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="105" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="106" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="107" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="108" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="109" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="110" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="111" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="112" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="113" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="114" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="115" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="116" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="117" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="118" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="119" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="120" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="121" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="122" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="123" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="124" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="125" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="126" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="127" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="128" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="129" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="130" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="131" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="132" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="133" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="134" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="135" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="136" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="137" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="138" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="139" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="140" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="141" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="142" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="143" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="144" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="145" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="146" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="16">
+    <mergeCell ref="C88:D88"/>
+    <mergeCell ref="C89:D89"/>
+    <mergeCell ref="A7:F7"/>
+    <mergeCell ref="H7:K7"/>
+    <mergeCell ref="C84:D84"/>
+    <mergeCell ref="C85:D85"/>
+    <mergeCell ref="C86:D86"/>
+    <mergeCell ref="C87:D87"/>
+    <mergeCell ref="K10:K14"/>
     <mergeCell ref="A6:F6"/>
     <mergeCell ref="H6:K6"/>
     <mergeCell ref="A1:K1"/>
@@ -2746,14 +4346,6 @@
     <mergeCell ref="A3:K3"/>
     <mergeCell ref="A4:K4"/>
     <mergeCell ref="A5:K5"/>
-    <mergeCell ref="C43:D43"/>
-    <mergeCell ref="C44:D44"/>
-    <mergeCell ref="A7:F7"/>
-    <mergeCell ref="H7:K7"/>
-    <mergeCell ref="C39:D39"/>
-    <mergeCell ref="C40:D40"/>
-    <mergeCell ref="C41:D41"/>
-    <mergeCell ref="C42:D42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
@@ -2763,5 +4355,6 @@
 Er. Milan Phuyal&amp;RApproved By:
 Er. Prakash Singh Saud</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
little edite3d in om shanti mandir for provisional sum amount
</commit_message>
<xml_diff>
--- a/ofc/estimates/Om shanti mandir/ૐ शान्ति भवन निर्माण तथा मर्मत.xlsx
+++ b/ofc/estimates/Om shanti mandir/ૐ शान्ति भवन निर्माण तथा मर्मत.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\081_082\ofc\ofc\estimates\Om shanti mandir\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\081-082\ofc\estimates\Om shanti mandir\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="WCR" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Sheet4 (2)'!$1:$8</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">WCR!$1:$12</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -490,9 +490,6 @@
     <t>set</t>
   </si>
   <si>
-    <t>Date:2081/06/08</t>
-  </si>
-  <si>
     <t>sqm</t>
   </si>
   <si>
@@ -607,14 +604,17 @@
   <si>
     <t>Item 134 from civil rate</t>
   </si>
+  <si>
+    <t>Date:2081/09/11</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
@@ -851,7 +851,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="94">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -861,7 +861,7 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -881,14 +881,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -897,7 +897,7 @@
     <xf numFmtId="1" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -922,7 +922,7 @@
     <xf numFmtId="1" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -957,7 +957,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -965,7 +965,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -980,7 +980,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -996,7 +996,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1009,7 +1009,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1072,12 +1078,6 @@
     </xf>
     <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1651,106 +1651,106 @@
       <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.28515625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-    </row>
-    <row r="2" spans="1:11" ht="24.6" x14ac:dyDescent="0.4">
-      <c r="A2" s="70" t="s">
+      <c r="B1" s="71"/>
+      <c r="C1" s="71"/>
+      <c r="D1" s="71"/>
+      <c r="E1" s="71"/>
+      <c r="F1" s="71"/>
+      <c r="G1" s="71"/>
+      <c r="H1" s="71"/>
+      <c r="I1" s="71"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="71"/>
+    </row>
+    <row r="2" spans="1:11" ht="25.5" x14ac:dyDescent="0.35">
+      <c r="A2" s="72" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="70"/>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-    </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="s">
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+    </row>
+    <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-    </row>
-    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="71" t="s">
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+    </row>
+    <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-    </row>
-    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="A5" s="72" t="s">
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+    </row>
+    <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="74" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="72"/>
-      <c r="D5" s="72"/>
-      <c r="E5" s="72"/>
-      <c r="F5" s="72"/>
-      <c r="G5" s="72"/>
-      <c r="H5" s="72"/>
-      <c r="I5" s="72"/>
-      <c r="J5" s="72"/>
-      <c r="K5" s="72"/>
-    </row>
-    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.35">
+      <c r="B5" s="74"/>
+      <c r="C5" s="74"/>
+      <c r="D5" s="74"/>
+      <c r="E5" s="74"/>
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+      <c r="H5" s="74"/>
+      <c r="I5" s="74"/>
+      <c r="J5" s="74"/>
+      <c r="K5" s="74"/>
+    </row>
+    <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="67" t="e">
+      <c r="C6" s="69" t="e">
         <f>F18</f>
         <v>#REF!</v>
       </c>
-      <c r="D6" s="68"/>
+      <c r="D6" s="70"/>
       <c r="E6" s="9"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
@@ -1758,90 +1758,90 @@
         <v>20</v>
       </c>
       <c r="I6" s="8"/>
-      <c r="J6" s="67" t="e">
+      <c r="J6" s="69" t="e">
         <f>I18</f>
         <v>#REF!</v>
       </c>
-      <c r="K6" s="68"/>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="K6" s="70"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="26" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="10"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="I7" s="77" t="s">
+      <c r="F7" s="78"/>
+      <c r="G7" s="78"/>
+      <c r="I7" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="77"/>
-      <c r="K7" s="77"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="75" t="e">
+      <c r="J7" s="79"/>
+      <c r="K7" s="79"/>
+    </row>
+    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="77" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="I8" s="78" t="s">
+      <c r="B8" s="77"/>
+      <c r="C8" s="77"/>
+      <c r="D8" s="77"/>
+      <c r="E8" s="77"/>
+      <c r="F8" s="77"/>
+      <c r="I8" s="80" t="s">
         <v>38</v>
       </c>
-      <c r="J8" s="78"/>
-      <c r="K8" s="78"/>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="79" t="e">
+      <c r="J8" s="80"/>
+      <c r="K8" s="80"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" s="81" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
-      <c r="B9" s="79"/>
-      <c r="C9" s="79"/>
-      <c r="D9" s="79"/>
-      <c r="E9" s="79"/>
-      <c r="F9" s="79"/>
-      <c r="I9" s="78" t="s">
+      <c r="B9" s="81"/>
+      <c r="C9" s="81"/>
+      <c r="D9" s="81"/>
+      <c r="E9" s="81"/>
+      <c r="F9" s="81"/>
+      <c r="I9" s="80" t="s">
         <v>39</v>
       </c>
-      <c r="J9" s="78"/>
-      <c r="K9" s="78"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="73" t="s">
+      <c r="J9" s="80"/>
+      <c r="K9" s="80"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="73" t="s">
+      <c r="B11" s="75" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="73" t="s">
+      <c r="C11" s="75" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="80" t="s">
+      <c r="D11" s="82" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="80"/>
-      <c r="F11" s="80"/>
-      <c r="G11" s="80" t="s">
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="80"/>
-      <c r="I11" s="80"/>
-      <c r="J11" s="73" t="s">
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="75" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="74" t="s">
+      <c r="K11" s="76" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="73"/>
-      <c r="B12" s="73"/>
-      <c r="C12" s="73"/>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" s="75"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
       <c r="D12" s="11" t="s">
         <v>26</v>
       </c>
@@ -1860,10 +1860,10 @@
       <c r="I12" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="73"/>
-      <c r="K12" s="74"/>
-    </row>
-    <row r="13" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="J12" s="75"/>
+      <c r="K12" s="76"/>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="27" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1906,7 +1906,7 @@
       </c>
       <c r="K13" s="14"/>
     </row>
-    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" s="1" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="27"/>
       <c r="B14" s="33" t="e">
         <f>#REF!</f>
@@ -1928,7 +1928,7 @@
       <c r="J14" s="28"/>
       <c r="K14" s="14"/>
     </row>
-    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="29"/>
       <c r="B15" s="29"/>
       <c r="C15" s="12"/>
@@ -1941,7 +1941,7 @@
       <c r="J15" s="28"/>
       <c r="K15" s="14"/>
     </row>
-    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="27" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
@@ -1984,7 +1984,7 @@
       </c>
       <c r="K16" s="14"/>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="29"/>
       <c r="B17" s="29"/>
       <c r="C17" s="12"/>
@@ -1997,7 +1997,7 @@
       <c r="J17" s="28"/>
       <c r="K17" s="14"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="5"/>
       <c r="B18" s="6" t="s">
         <v>16</v>
@@ -2060,134 +2060,134 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="3" max="3" width="4.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5546875" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31.28515625" customWidth="1"/>
+    <col min="3" max="3" width="4.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" customWidth="1"/>
     <col min="6" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="9.44140625" customWidth="1"/>
+    <col min="7" max="7" width="9.42578125" customWidth="1"/>
     <col min="8" max="8" width="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.88671875" customWidth="1"/>
-    <col min="10" max="10" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.85546875" customWidth="1"/>
+    <col min="10" max="10" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="82" t="s">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
-      <c r="F1" s="82"/>
-      <c r="G1" s="82"/>
-      <c r="H1" s="82"/>
-      <c r="I1" s="82"/>
-      <c r="J1" s="82"/>
-      <c r="K1" s="82"/>
-    </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="83" t="s">
+      <c r="B1" s="84"/>
+      <c r="C1" s="84"/>
+      <c r="D1" s="84"/>
+      <c r="E1" s="84"/>
+      <c r="F1" s="84"/>
+      <c r="G1" s="84"/>
+      <c r="H1" s="84"/>
+      <c r="I1" s="84"/>
+      <c r="J1" s="84"/>
+      <c r="K1" s="84"/>
+    </row>
+    <row r="2" spans="1:19" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-    </row>
-    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="71" t="s">
+      <c r="B2" s="85"/>
+      <c r="C2" s="85"/>
+      <c r="D2" s="85"/>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="85"/>
+      <c r="I2" s="85"/>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+    </row>
+    <row r="3" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="71"/>
-      <c r="C3" s="71"/>
-      <c r="D3" s="71"/>
-      <c r="E3" s="71"/>
-      <c r="F3" s="71"/>
-      <c r="G3" s="71"/>
-      <c r="H3" s="71"/>
-      <c r="I3" s="71"/>
-      <c r="J3" s="71"/>
-      <c r="K3" s="71"/>
-    </row>
-    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="71" t="s">
+      <c r="B3" s="73"/>
+      <c r="C3" s="73"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
+      <c r="I3" s="73"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="73"/>
+    </row>
+    <row r="4" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="71"/>
-      <c r="C4" s="71"/>
-      <c r="D4" s="71"/>
-      <c r="E4" s="71"/>
-      <c r="F4" s="71"/>
-      <c r="G4" s="71"/>
-      <c r="H4" s="71"/>
-      <c r="I4" s="71"/>
-      <c r="J4" s="71"/>
-      <c r="K4" s="71"/>
-    </row>
-    <row r="5" spans="1:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A5" s="84" t="s">
+      <c r="B4" s="73"/>
+      <c r="C4" s="73"/>
+      <c r="D4" s="73"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
+      <c r="I4" s="73"/>
+      <c r="J4" s="73"/>
+      <c r="K4" s="73"/>
+    </row>
+    <row r="5" spans="1:19" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A5" s="86" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
-    </row>
-    <row r="6" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="75" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="75"/>
-      <c r="C6" s="75"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+    </row>
+    <row r="6" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="77"/>
+      <c r="C6" s="77"/>
+      <c r="D6" s="77"/>
+      <c r="E6" s="77"/>
+      <c r="F6" s="77"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="81" t="s">
+      <c r="H6" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="I6" s="81"/>
-      <c r="J6" s="81"/>
-      <c r="K6" s="81"/>
-    </row>
-    <row r="7" spans="1:19" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="86" t="s">
+      <c r="I6" s="83"/>
+      <c r="J6" s="83"/>
+      <c r="K6" s="83"/>
+    </row>
+    <row r="7" spans="1:19" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="86"/>
-      <c r="C7" s="86"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="86"/>
-      <c r="F7" s="86"/>
+      <c r="B7" s="88"/>
+      <c r="C7" s="88"/>
+      <c r="D7" s="88"/>
+      <c r="E7" s="88"/>
+      <c r="F7" s="88"/>
       <c r="G7" s="3"/>
-      <c r="H7" s="87" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="87"/>
-      <c r="J7" s="87"/>
-      <c r="K7" s="87"/>
-    </row>
-    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="89" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" s="89"/>
+      <c r="J7" s="89"/>
+      <c r="K7" s="89"/>
+    </row>
+    <row r="8" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
@@ -2222,12 +2222,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="1" customFormat="1" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" s="1" customFormat="1" ht="54.75" x14ac:dyDescent="0.25">
       <c r="A9" s="63">
         <v>1</v>
       </c>
       <c r="B9" s="64" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="64"/>
       <c r="D9" s="40"/>
@@ -2239,10 +2239,10 @@
       <c r="J9" s="45"/>
       <c r="K9" s="29"/>
     </row>
-    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="18"/>
       <c r="B10" s="38" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C10" s="37">
         <v>1</v>
@@ -2264,7 +2264,7 @@
       <c r="I10" s="41"/>
       <c r="J10" s="41"/>
       <c r="K10" s="91" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="M10" s="25"/>
       <c r="N10" s="1"/>
@@ -2274,10 +2274,10 @@
       <c r="R10" s="25"/>
       <c r="S10" s="25"/>
     </row>
-    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="18"/>
       <c r="B11" s="38" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C11" s="37">
         <v>1</v>
@@ -2307,10 +2307,10 @@
       <c r="R11" s="25"/>
       <c r="S11" s="25"/>
     </row>
-    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="18"/>
       <c r="B12" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C12" s="37">
         <v>-6</v>
@@ -2338,7 +2338,7 @@
       <c r="R12" s="25"/>
       <c r="S12" s="25"/>
     </row>
-    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="18"/>
       <c r="B13" s="38"/>
       <c r="C13" s="37">
@@ -2367,7 +2367,7 @@
       <c r="R13" s="25"/>
       <c r="S13" s="25"/>
     </row>
-    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="18"/>
       <c r="B14" s="38"/>
       <c r="C14" s="37">
@@ -2396,7 +2396,7 @@
       <c r="R14" s="25"/>
       <c r="S14" s="25"/>
     </row>
-    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="18"/>
       <c r="B15" s="38" t="s">
         <v>41</v>
@@ -2410,7 +2410,7 @@
         <v>17.972823016200429</v>
       </c>
       <c r="H15" s="41" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I15" s="41">
         <v>2807.39</v>
@@ -2428,7 +2428,7 @@
       <c r="R15" s="25"/>
       <c r="S15" s="25"/>
     </row>
-    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="18"/>
       <c r="B16" s="38" t="s">
         <v>40</v>
@@ -2453,7 +2453,7 @@
       <c r="R16" s="25"/>
       <c r="S16" s="25"/>
     </row>
-    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18"/>
       <c r="B17" s="38"/>
       <c r="C17" s="37"/>
@@ -2473,12 +2473,12 @@
       <c r="R17" s="25"/>
       <c r="S17" s="25"/>
     </row>
-    <row r="18" spans="1:19" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="18">
         <v>2</v>
       </c>
-      <c r="B18" s="89" t="s">
-        <v>67</v>
+      <c r="B18" s="67" t="s">
+        <v>66</v>
       </c>
       <c r="C18" s="37"/>
       <c r="D18" s="39"/>
@@ -2497,10 +2497,10 @@
       <c r="R18" s="25"/>
       <c r="S18" s="25"/>
     </row>
-    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="18"/>
       <c r="B19" s="38" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="37">
         <v>1</v>
@@ -2524,7 +2524,7 @@
       <c r="R19" s="25"/>
       <c r="S19" s="25"/>
     </row>
-    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="18"/>
       <c r="B20" s="38" t="s">
         <v>41</v>
@@ -2556,7 +2556,7 @@
       <c r="R20" s="25"/>
       <c r="S20" s="25"/>
     </row>
-    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="18"/>
       <c r="B21" s="38" t="s">
         <v>40</v>
@@ -2581,7 +2581,7 @@
       <c r="R21" s="25"/>
       <c r="S21" s="25"/>
     </row>
-    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="18"/>
       <c r="B22" s="38"/>
       <c r="C22" s="37"/>
@@ -2601,12 +2601,12 @@
       <c r="R22" s="25"/>
       <c r="S22" s="25"/>
     </row>
-    <row r="23" spans="1:19" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="18">
         <v>3</v>
       </c>
       <c r="B23" s="65" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C23" s="37"/>
       <c r="D23" s="39"/>
@@ -2625,10 +2625,10 @@
       <c r="R23" s="25"/>
       <c r="S23" s="25"/>
     </row>
-    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="18"/>
       <c r="B24" s="38" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C24" s="37">
         <v>1</v>
@@ -2652,7 +2652,7 @@
       <c r="R24" s="25"/>
       <c r="S24" s="25"/>
     </row>
-    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="18"/>
       <c r="B25" s="38" t="s">
         <v>41</v>
@@ -2666,7 +2666,7 @@
         <v>1</v>
       </c>
       <c r="H25" s="41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I25" s="41">
         <v>1798</v>
@@ -2684,7 +2684,7 @@
       <c r="R25" s="25"/>
       <c r="S25" s="25"/>
     </row>
-    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="18"/>
       <c r="B26" s="38" t="s">
         <v>40</v>
@@ -2709,7 +2709,7 @@
       <c r="R26" s="25"/>
       <c r="S26" s="25"/>
     </row>
-    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="18"/>
       <c r="B27" s="38"/>
       <c r="C27" s="37"/>
@@ -2729,12 +2729,12 @@
       <c r="R27" s="25"/>
       <c r="S27" s="25"/>
     </row>
-    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="18">
         <v>4</v>
       </c>
       <c r="B28" s="65" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C28" s="37"/>
       <c r="D28" s="39"/>
@@ -2753,10 +2753,10 @@
       <c r="R28" s="25"/>
       <c r="S28" s="25"/>
     </row>
-    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="18"/>
       <c r="B29" s="38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C29" s="37">
         <v>1</v>
@@ -2782,7 +2782,7 @@
       <c r="R29" s="25"/>
       <c r="S29" s="25"/>
     </row>
-    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="18"/>
       <c r="B30" s="38" t="s">
         <v>41</v>
@@ -2796,7 +2796,7 @@
         <v>2</v>
       </c>
       <c r="H30" s="41" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="I30" s="41">
         <f>1230/40</f>
@@ -2815,7 +2815,7 @@
       <c r="R30" s="25"/>
       <c r="S30" s="25"/>
     </row>
-    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="18"/>
       <c r="B31" s="38" t="s">
         <v>40</v>
@@ -2840,7 +2840,7 @@
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
     </row>
-    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="18"/>
       <c r="B32" s="38"/>
       <c r="C32" s="37"/>
@@ -2860,12 +2860,12 @@
       <c r="R32" s="25"/>
       <c r="S32" s="25"/>
     </row>
-    <row r="33" spans="1:19" s="1" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" s="1" customFormat="1" ht="28.5" x14ac:dyDescent="0.25">
       <c r="A33" s="18">
         <v>5</v>
       </c>
       <c r="B33" s="66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" s="29"/>
       <c r="D33" s="40"/>
@@ -2880,10 +2880,10 @@
       <c r="R33" s="35"/>
       <c r="S33" s="35"/>
     </row>
-    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="18"/>
       <c r="B34" s="38" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C34" s="37">
         <v>1</v>
@@ -2907,7 +2907,7 @@
       <c r="R34" s="25"/>
       <c r="S34" s="25"/>
     </row>
-    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18"/>
       <c r="B35" s="38" t="s">
         <v>41</v>
@@ -2939,7 +2939,7 @@
       <c r="R35" s="25"/>
       <c r="S35" s="25"/>
     </row>
-    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="18"/>
       <c r="B36" s="38" t="s">
         <v>40</v>
@@ -2964,7 +2964,7 @@
       <c r="R36" s="25"/>
       <c r="S36" s="25"/>
     </row>
-    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="18"/>
       <c r="B37" s="38"/>
       <c r="C37" s="37"/>
@@ -2984,12 +2984,12 @@
       <c r="R37" s="25"/>
       <c r="S37" s="25"/>
     </row>
-    <row r="38" spans="1:19" s="1" customFormat="1" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" s="1" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
       <c r="A38" s="18">
         <v>6</v>
       </c>
       <c r="B38" s="66" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C38" s="29"/>
       <c r="D38" s="40"/>
@@ -3004,10 +3004,10 @@
       <c r="R38" s="35"/>
       <c r="S38" s="35"/>
     </row>
-    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="18"/>
       <c r="B39" s="38" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C39" s="37">
         <v>1</v>
@@ -3031,7 +3031,7 @@
       <c r="R39" s="25"/>
       <c r="S39" s="25"/>
     </row>
-    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="18"/>
       <c r="B40" s="38" t="s">
         <v>41</v>
@@ -3063,7 +3063,7 @@
       <c r="R40" s="25"/>
       <c r="S40" s="25"/>
     </row>
-    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18"/>
       <c r="B41" s="38" t="s">
         <v>40</v>
@@ -3088,7 +3088,7 @@
       <c r="R41" s="25"/>
       <c r="S41" s="25"/>
     </row>
-    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18"/>
       <c r="B42" s="38"/>
       <c r="C42" s="37"/>
@@ -3108,12 +3108,12 @@
       <c r="R42" s="25"/>
       <c r="S42" s="25"/>
     </row>
-    <row r="43" spans="1:19" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A43" s="18">
         <v>7</v>
       </c>
-      <c r="B43" s="90" t="s">
-        <v>69</v>
+      <c r="B43" s="68" t="s">
+        <v>68</v>
       </c>
       <c r="C43" s="37"/>
       <c r="D43" s="39"/>
@@ -3132,10 +3132,10 @@
       <c r="R43" s="25"/>
       <c r="S43" s="25"/>
     </row>
-    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="18"/>
       <c r="B44" s="38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C44" s="37">
         <v>1</v>
@@ -3159,7 +3159,7 @@
       <c r="R44" s="25"/>
       <c r="S44" s="25"/>
     </row>
-    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="18"/>
       <c r="B45" s="38" t="s">
         <v>41</v>
@@ -3173,7 +3173,7 @@
         <v>1</v>
       </c>
       <c r="H45" s="41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="I45" s="41">
         <v>4425</v>
@@ -3191,7 +3191,7 @@
       <c r="R45" s="25"/>
       <c r="S45" s="25"/>
     </row>
-    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="18"/>
       <c r="B46" s="38" t="s">
         <v>40</v>
@@ -3216,7 +3216,7 @@
       <c r="R46" s="25"/>
       <c r="S46" s="25"/>
     </row>
-    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="18"/>
       <c r="B47" s="38"/>
       <c r="C47" s="37"/>
@@ -3236,12 +3236,12 @@
       <c r="R47" s="25"/>
       <c r="S47" s="25"/>
     </row>
-    <row r="48" spans="1:19" ht="42" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A48" s="18">
         <v>8</v>
       </c>
-      <c r="B48" s="90" t="s">
-        <v>70</v>
+      <c r="B48" s="68" t="s">
+        <v>69</v>
       </c>
       <c r="C48" s="37"/>
       <c r="D48" s="39"/>
@@ -3260,10 +3260,10 @@
       <c r="R48" s="25"/>
       <c r="S48" s="25"/>
     </row>
-    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="18"/>
       <c r="B49" s="38" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C49" s="37">
         <v>1</v>
@@ -3287,7 +3287,7 @@
       <c r="R49" s="25"/>
       <c r="S49" s="25"/>
     </row>
-    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="18"/>
       <c r="B50" s="38" t="s">
         <v>41</v>
@@ -3319,7 +3319,7 @@
       <c r="R50" s="25"/>
       <c r="S50" s="25"/>
     </row>
-    <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="18"/>
       <c r="B51" s="38" t="s">
         <v>40</v>
@@ -3344,7 +3344,7 @@
       <c r="R51" s="25"/>
       <c r="S51" s="25"/>
     </row>
-    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="18"/>
       <c r="B52" s="38"/>
       <c r="C52" s="37"/>
@@ -3364,12 +3364,12 @@
       <c r="R52" s="25"/>
       <c r="S52" s="25"/>
     </row>
-    <row r="53" spans="1:19" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" ht="43.5" x14ac:dyDescent="0.25">
       <c r="A53" s="18">
         <v>9</v>
       </c>
-      <c r="B53" s="90" t="s">
-        <v>71</v>
+      <c r="B53" s="68" t="s">
+        <v>70</v>
       </c>
       <c r="C53" s="37"/>
       <c r="D53" s="39"/>
@@ -3388,10 +3388,10 @@
       <c r="R53" s="25"/>
       <c r="S53" s="25"/>
     </row>
-    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="18"/>
       <c r="B54" s="38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C54" s="37">
         <v>1</v>
@@ -3415,7 +3415,7 @@
       <c r="R54" s="25"/>
       <c r="S54" s="25"/>
     </row>
-    <row r="55" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="18"/>
       <c r="B55" s="38" t="s">
         <v>41</v>
@@ -3447,7 +3447,7 @@
       <c r="R55" s="25"/>
       <c r="S55" s="25"/>
     </row>
-    <row r="56" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="18"/>
       <c r="B56" s="38" t="s">
         <v>40</v>
@@ -3472,7 +3472,7 @@
       <c r="R56" s="25"/>
       <c r="S56" s="25"/>
     </row>
-    <row r="57" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="18"/>
       <c r="B57" s="38"/>
       <c r="C57" s="37"/>
@@ -3492,12 +3492,12 @@
       <c r="R57" s="25"/>
       <c r="S57" s="25"/>
     </row>
-    <row r="58" spans="1:19" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A58" s="18">
         <v>10</v>
       </c>
-      <c r="B58" s="90" t="s">
-        <v>72</v>
+      <c r="B58" s="68" t="s">
+        <v>71</v>
       </c>
       <c r="C58" s="37"/>
       <c r="D58" s="39"/>
@@ -3516,10 +3516,10 @@
       <c r="R58" s="25"/>
       <c r="S58" s="25"/>
     </row>
-    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="18"/>
       <c r="B59" s="38" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C59" s="37">
         <v>1</v>
@@ -3543,7 +3543,7 @@
       <c r="R59" s="25"/>
       <c r="S59" s="25"/>
     </row>
-    <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="18"/>
       <c r="B60" s="38" t="s">
         <v>41</v>
@@ -3575,7 +3575,7 @@
       <c r="R60" s="25"/>
       <c r="S60" s="25"/>
     </row>
-    <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="18"/>
       <c r="B61" s="38" t="s">
         <v>40</v>
@@ -3600,7 +3600,7 @@
       <c r="R61" s="25"/>
       <c r="S61" s="25"/>
     </row>
-    <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="18"/>
       <c r="B62" s="38"/>
       <c r="C62" s="37"/>
@@ -3620,12 +3620,12 @@
       <c r="R62" s="25"/>
       <c r="S62" s="25"/>
     </row>
-    <row r="63" spans="1:19" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A63" s="18">
         <v>11</v>
       </c>
-      <c r="B63" s="90" t="s">
-        <v>73</v>
+      <c r="B63" s="68" t="s">
+        <v>72</v>
       </c>
       <c r="C63" s="37"/>
       <c r="D63" s="39"/>
@@ -3644,10 +3644,10 @@
       <c r="R63" s="25"/>
       <c r="S63" s="25"/>
     </row>
-    <row r="64" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="18"/>
       <c r="B64" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C64" s="37">
         <v>1</v>
@@ -3671,7 +3671,7 @@
       <c r="R64" s="25"/>
       <c r="S64" s="25"/>
     </row>
-    <row r="65" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="18"/>
       <c r="B65" s="38" t="s">
         <v>41</v>
@@ -3703,7 +3703,7 @@
       <c r="R65" s="25"/>
       <c r="S65" s="25"/>
     </row>
-    <row r="66" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="18"/>
       <c r="B66" s="38" t="s">
         <v>40</v>
@@ -3728,7 +3728,7 @@
       <c r="R66" s="25"/>
       <c r="S66" s="25"/>
     </row>
-    <row r="67" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A67" s="18"/>
       <c r="B67" s="38"/>
       <c r="C67" s="37"/>
@@ -3748,12 +3748,12 @@
       <c r="R67" s="25"/>
       <c r="S67" s="25"/>
     </row>
-    <row r="68" spans="1:19" ht="28.2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" ht="29.25" x14ac:dyDescent="0.25">
       <c r="A68" s="18">
         <v>12</v>
       </c>
-      <c r="B68" s="90" t="s">
-        <v>74</v>
+      <c r="B68" s="68" t="s">
+        <v>73</v>
       </c>
       <c r="C68" s="37"/>
       <c r="D68" s="39"/>
@@ -3772,10 +3772,10 @@
       <c r="R68" s="25"/>
       <c r="S68" s="25"/>
     </row>
-    <row r="69" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="18"/>
       <c r="B69" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C69" s="37">
         <v>1</v>
@@ -3799,7 +3799,7 @@
       <c r="R69" s="25"/>
       <c r="S69" s="25"/>
     </row>
-    <row r="70" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="18"/>
       <c r="B70" s="38" t="s">
         <v>41</v>
@@ -3831,7 +3831,7 @@
       <c r="R70" s="25"/>
       <c r="S70" s="25"/>
     </row>
-    <row r="71" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="18"/>
       <c r="B71" s="38" t="s">
         <v>40</v>
@@ -3856,7 +3856,7 @@
       <c r="R71" s="25"/>
       <c r="S71" s="25"/>
     </row>
-    <row r="72" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="18"/>
       <c r="B72" s="38"/>
       <c r="C72" s="37"/>
@@ -3876,12 +3876,12 @@
       <c r="R72" s="25"/>
       <c r="S72" s="25"/>
     </row>
-    <row r="73" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="18">
         <v>13</v>
       </c>
-      <c r="B73" s="90" t="s">
-        <v>75</v>
+      <c r="B73" s="68" t="s">
+        <v>74</v>
       </c>
       <c r="C73" s="37"/>
       <c r="D73" s="39"/>
@@ -3900,10 +3900,10 @@
       <c r="R73" s="25"/>
       <c r="S73" s="25"/>
     </row>
-    <row r="74" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="18"/>
       <c r="B74" s="38" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C74" s="37">
         <v>1</v>
@@ -3927,7 +3927,7 @@
       <c r="R74" s="25"/>
       <c r="S74" s="25"/>
     </row>
-    <row r="75" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="18"/>
       <c r="B75" s="38" t="s">
         <v>41</v>
@@ -3959,7 +3959,7 @@
       <c r="R75" s="25"/>
       <c r="S75" s="25"/>
     </row>
-    <row r="76" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="18"/>
       <c r="B76" s="38" t="s">
         <v>40</v>
@@ -3984,7 +3984,7 @@
       <c r="R76" s="25"/>
       <c r="S76" s="25"/>
     </row>
-    <row r="77" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="18"/>
       <c r="B77" s="38"/>
       <c r="C77" s="37"/>
@@ -4004,12 +4004,12 @@
       <c r="R77" s="25"/>
       <c r="S77" s="25"/>
     </row>
-    <row r="78" spans="1:19" ht="19.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:19" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="18">
         <v>14</v>
       </c>
       <c r="B78" s="30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C78" s="19">
         <v>1</v>
@@ -4025,11 +4025,11 @@
         <v>31</v>
       </c>
       <c r="I78" s="23">
-        <v>12000</v>
+        <v>10000</v>
       </c>
       <c r="J78" s="34">
         <f>G78*I78</f>
-        <v>12000</v>
+        <v>10000</v>
       </c>
       <c r="K78" s="21"/>
       <c r="M78" s="25"/>
@@ -4040,7 +4040,7 @@
       <c r="R78" s="25"/>
       <c r="S78" s="25"/>
     </row>
-    <row r="79" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="41"/>
       <c r="B79" s="38"/>
       <c r="C79" s="43"/>
@@ -4053,7 +4053,7 @@
       <c r="J79" s="45"/>
       <c r="K79" s="37"/>
     </row>
-    <row r="80" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="18">
         <v>15</v>
       </c>
@@ -4089,7 +4089,7 @@
       <c r="R80" s="25"/>
       <c r="S80" s="25"/>
     </row>
-    <row r="81" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="18"/>
       <c r="B81" s="24"/>
       <c r="C81" s="19"/>
@@ -4109,7 +4109,7 @@
       <c r="R81" s="25"/>
       <c r="S81" s="25"/>
     </row>
-    <row r="82" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A82" s="41"/>
       <c r="B82" s="46" t="s">
         <v>17</v>
@@ -4123,11 +4123,11 @@
       <c r="I82" s="42"/>
       <c r="J82" s="42">
         <f>SUM(J9:J80)</f>
-        <v>117578.08333909372</v>
+        <v>115578.08333909372</v>
       </c>
       <c r="K82" s="37"/>
     </row>
-    <row r="83" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A83" s="58"/>
       <c r="B83" s="61"/>
       <c r="C83" s="62"/>
@@ -4140,16 +4140,16 @@
       <c r="J83" s="60"/>
       <c r="K83" s="57"/>
     </row>
-    <row r="84" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="50"/>
       <c r="B84" s="29" t="s">
         <v>27</v>
       </c>
-      <c r="C84" s="85">
+      <c r="C84" s="87">
         <f>J82</f>
-        <v>117578.08333909372</v>
-      </c>
-      <c r="D84" s="85"/>
+        <v>115578.08333909372</v>
+      </c>
+      <c r="D84" s="87"/>
       <c r="E84" s="40">
         <v>100</v>
       </c>
@@ -4160,15 +4160,15 @@
       <c r="J84" s="54"/>
       <c r="K84" s="55"/>
     </row>
-    <row r="85" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A85" s="56"/>
       <c r="B85" s="29" t="s">
         <v>32</v>
       </c>
-      <c r="C85" s="88">
+      <c r="C85" s="90">
         <v>100000</v>
       </c>
-      <c r="D85" s="88"/>
+      <c r="D85" s="90"/>
       <c r="E85" s="40"/>
       <c r="F85" s="49"/>
       <c r="G85" s="48"/>
@@ -4177,19 +4177,19 @@
       <c r="J85" s="48"/>
       <c r="K85" s="49"/>
     </row>
-    <row r="86" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A86" s="56"/>
       <c r="B86" s="29" t="s">
         <v>33</v>
       </c>
-      <c r="C86" s="88">
+      <c r="C86" s="90">
         <f>C85-C88-C89</f>
         <v>95000</v>
       </c>
-      <c r="D86" s="88"/>
+      <c r="D86" s="90"/>
       <c r="E86" s="40">
         <f>C86/C84*100</f>
-        <v>80.797370821244968</v>
+        <v>82.195514283863119</v>
       </c>
       <c r="F86" s="49"/>
       <c r="G86" s="48"/>
@@ -4198,19 +4198,19 @@
       <c r="J86" s="48"/>
       <c r="K86" s="49"/>
     </row>
-    <row r="87" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A87" s="56"/>
       <c r="B87" s="29" t="s">
         <v>34</v>
       </c>
-      <c r="C87" s="85">
+      <c r="C87" s="87">
         <f>C84-C86</f>
-        <v>22578.083339093719</v>
-      </c>
-      <c r="D87" s="85"/>
+        <v>20578.083339093719</v>
+      </c>
+      <c r="D87" s="87"/>
       <c r="E87" s="40">
         <f>100-E86</f>
-        <v>19.202629178755032</v>
+        <v>17.804485716136881</v>
       </c>
       <c r="F87" s="49"/>
       <c r="G87" s="48"/>
@@ -4219,16 +4219,16 @@
       <c r="J87" s="48"/>
       <c r="K87" s="49"/>
     </row>
-    <row r="88" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A88" s="56"/>
       <c r="B88" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="C88" s="85">
+      <c r="C88" s="87">
         <f>C85*0.03</f>
         <v>3000</v>
       </c>
-      <c r="D88" s="85"/>
+      <c r="D88" s="87"/>
       <c r="E88" s="40">
         <v>3</v>
       </c>
@@ -4239,16 +4239,16 @@
       <c r="J88" s="48"/>
       <c r="K88" s="49"/>
     </row>
-    <row r="89" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A89" s="56"/>
       <c r="B89" s="29" t="s">
         <v>36</v>
       </c>
-      <c r="C89" s="85">
+      <c r="C89" s="87">
         <f>C85*0.02</f>
         <v>2000</v>
       </c>
-      <c r="D89" s="85"/>
+      <c r="D89" s="87"/>
       <c r="E89" s="40">
         <v>2</v>
       </c>
@@ -4259,7 +4259,7 @@
       <c r="J89" s="48"/>
       <c r="K89" s="49"/>
     </row>
-    <row r="90" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="57"/>
       <c r="B90" s="57"/>
       <c r="C90" s="57"/>
@@ -4272,62 +4272,62 @@
       <c r="J90" s="57"/>
       <c r="K90" s="57"/>
     </row>
-    <row r="91" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="92" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="93" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="94" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="95" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="96" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="97" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="98" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="100" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="101" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="102" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="103" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="104" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="105" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="106" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="107" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="108" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="109" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="110" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="111" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="112" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="113" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="114" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="115" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="116" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="117" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="118" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="119" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="120" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="121" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="122" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="123" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="124" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="125" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="126" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="127" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="128" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="129" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="130" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="131" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="132" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="133" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="134" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="135" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="136" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="137" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="138" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="139" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="140" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="141" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="142" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="143" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="144" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="145" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="146" s="36" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="97" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="98" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="99" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="100" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="101" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="102" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="103" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="104" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="105" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="106" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="107" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="108" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="109" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="110" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="111" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="112" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="113" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="114" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="115" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="116" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="117" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="118" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="119" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="120" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="121" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="122" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="123" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="124" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="125" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="126" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="127" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="128" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="129" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="130" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="131" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="132" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="133" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="134" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="135" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="136" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="137" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="138" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="139" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="140" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="141" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="142" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="143" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="144" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="145" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="146" s="36" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="16">
     <mergeCell ref="C88:D88"/>
@@ -4350,10 +4350,7 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;LPrepared By:
-Kristal Suwal&amp;CChecked By:
-Er. Milan Phuyal&amp;RApproved By:
-Er. Prakash Singh Saud</oddFooter>
+    <oddFooter>&amp;LPrepared By:&amp;CChecked By:&amp;RApproved By:</oddFooter>
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>

</xml_diff>